<commit_message>
Unevaluated Resutls of Gemini and GPT
</commit_message>
<xml_diff>
--- a/Enslaved/Original/NEN/Results/Enslaved_NEN_Gemini_results_Unevaluated.xlsx
+++ b/Enslaved/Original/NEN/Results/Enslaved_NEN_Gemini_results_Unevaluated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisdavisj/graph-rag-iswc-2025/util-scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisdavisj/knowledge-conceptualization-graphrag/util-scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8E5447-2743-2D4D-9A2C-AF78516108FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAE6BD9-A1B0-D741-B9F6-8301C6FF0346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,50 +48,71 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-# Cannot answer this question with the provided schema.
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+SELECT ?enslavedPerson
+WHERE {
+  ?enslavedPersonRecord rdf:type/rdfs:subClassOf* &lt;AgentRecord&gt; .
+  ?enslavedPersonRecord providesParticipantRole ?participantRole .
+  ?participantRole hasParticipantRoleType "enslaved" . # Assuming "enslaved" is a value in ParticipantRoleTypes.txt
+  ?event rdf:type/rdfs:subClassOf* &lt;Event&gt; .
+  ?event providesParticipantRole ?participantRole .
+  ?event hasTemporalExtent ?temporalExtent .
+  ?temporalExtent contains ?date .
+  FILTER (YEAR(?date) &gt;= 1700 &amp;&amp; YEAR(?date) &lt; 1800) #Example Century
+  #Assuming location is tied to the Event
+  ?event hasLocation ?location .
+  ?location hasName "County X" . #Assuming "County X" is a value for location
+}
 ```</t>
   </si>
   <si>
@@ -109,7 +130,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\n# Cannot answer this question with the provided schema.\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?enslavedPerson\nWHERE {\n  ?enslavedPersonRecord rdf:type/rdfs:subClassOf* &lt;AgentRecord&gt; .\n  ?enslavedPersonRecord providesParticipantRole ?participantRole .\n  ?participantRole hasParticipantRoleType \"enslaved\" . # Assuming \"enslaved\" is a value in ParticipantRoleTypes.txt\n\n  ?event rdf:type/rdfs:subClassOf* &lt;Event&gt; .\n  ?event providesParticipantRole ?participantRole .\n\n  ?event hasTemporalExtent ?temporalExtent .\n  ?temporalExtent contains ?date .\n  FILTER (YEAR(?date) &gt;= 1700 &amp;&amp; YEAR(?date) &lt; 1800) #Example Century\n\n  #Assuming location is tied to the Event\n  ?event hasLocation ?location .\n  ?location hasName \"County X\" . #Assuming \"County X\" is a value for location\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -118,7 +139,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.2633419930934906,
+            "avg_logprobs": -0.1388097738290762,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -132,24 +153,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 16,
+        "candidates_token_count": 308,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 16
+                "token_count": 308
             }
         ],
-        "prompt_token_count": 674,
+        "prompt_token_count": 692,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 674
+                "token_count": 692
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 690
+        "total_token_count": 1000
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -170,63 +191,80 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
 SELECT ?agent ?gender ?ethnicity ?location WHERE {
-  ?agent rdf:type Agent .
+  ?agent rdf:type &lt;http://example.org/Agent&gt; .
   OPTIONAL {
-    ?agent hasSexRecord ?sexRecord .
-    ?sexRecord hasValue ?gender .
+    ?agent ?genderProperty ?genderRecord .
+    ?genderRecord rdf:type &lt;http://example.org/SexRecord&gt; .
+    ?genderRecord &lt;http://example.org/hasValue&gt; ?gender .
   }
   OPTIONAL {
-    ?agent hasEthnicityRecord ?ethnicityRecord .
-    ?ethnicityRecord hasValue ?ethnicity .
+    ?agent ?ethnicityProperty ?ethnicityRecord .
+    ?ethnicityRecord rdf:type &lt;http://example.org/EthnicityRecord&gt; . # Assuming EthnicityRecord exists
+    ?ethnicityRecord &lt;http://example.org/hasValue&gt; ?ethnicity .
   }
   OPTIONAL {
-    ?agent hasLocationRecord ?locationRecord .
-    ?locationRecord hasValue ?location .
+    ?agent ?locationProperty ?locationValue .
+    ?locationValue rdf:type &lt;http://example.org/Location&gt; . # Assuming Location class exists
+    ?locationValue &lt;http://example.org/hasName&gt; ?location . # Assuming Location has a name
   }
+  FILTER NOT EXISTS {
+     ?agent rdf:type &lt;http://example.org/NonEnslavedAgent&gt;. #Ensuring only enslaved people are returned
+  }
+  VALUES (?genderProperty) { (&lt;http://example.org/hasAgentRecord&gt;) }
+  VALUES (?ethnicityProperty) { (&lt;http://example.org/hasAgentRecord&gt;) }
+  VALUES (?locationProperty) { (&lt;http://example.org/locatedAt&gt;) }
 }
 ```</t>
   </si>
@@ -245,7 +283,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT ?agent ?gender ?ethnicity ?location WHERE {\n  ?agent rdf:type Agent .\n  OPTIONAL {\n    ?agent hasSexRecord ?sexRecord .\n    ?sexRecord hasValue ?gender .\n  }\n  OPTIONAL {\n    ?agent hasEthnicityRecord ?ethnicityRecord .\n    ?ethnicityRecord hasValue ?ethnicity .\n  }\n  OPTIONAL {\n    ?agent hasLocationRecord ?locationRecord .\n    ?locationRecord hasValue ?location .\n  }\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?agent ?gender ?ethnicity ?location WHERE {\n  ?agent rdf:type &lt;http://example.org/Agent&gt; .\n  OPTIONAL {\n    ?agent ?genderProperty ?genderRecord .\n    ?genderRecord rdf:type &lt;http://example.org/SexRecord&gt; .\n    ?genderRecord &lt;http://example.org/hasValue&gt; ?gender .\n  }\n  OPTIONAL {\n    ?agent ?ethnicityProperty ?ethnicityRecord .\n    ?ethnicityRecord rdf:type &lt;http://example.org/EthnicityRecord&gt; . # Assuming EthnicityRecord exists\n    ?ethnicityRecord &lt;http://example.org/hasValue&gt; ?ethnicity .\n  }\n  OPTIONAL {\n    ?agent ?locationProperty ?locationValue .\n    ?locationValue rdf:type &lt;http://example.org/Location&gt; . # Assuming Location class exists\n    ?locationValue &lt;http://example.org/hasName&gt; ?location . # Assuming Location has a name\n  }\n  FILTER NOT EXISTS {\n     ?agent rdf:type &lt;http://example.org/NonEnslavedAgent&gt;. #Ensuring only enslaved people are returned\n  }\n  VALUES (?genderProperty) { (&lt;http://example.org/hasAgentRecord&gt;) }\n  VALUES (?ethnicityProperty) { (&lt;http://example.org/hasAgentRecord&gt;) }\n  VALUES (?locationProperty) { (&lt;http://example.org/locatedAt&gt;) }\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -254,7 +292,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.01615224140030997,
+            "avg_logprobs": -0.067376633244623,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -268,24 +306,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 112,
+        "candidates_token_count": 413,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 112
+                "token_count": 413
             }
         ],
-        "prompt_token_count": 687,
+        "prompt_token_count": 705,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 687
+                "token_count": 705
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 799
+        "total_token_count": 1118
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -306,45 +344,49 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
@@ -355,15 +397,14 @@
 PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
 SELECT ?place ?year ?populationCount
 WHERE {
-  ?event rdf:type &lt;Event&gt; .
-  ?event &lt;hasPlace&gt; ?place .
-  ?event time:hasTime ?temporalEntity .
-  ?temporalEntity time:hasBeginning ?timeInstant .
-  ?timeInstant time:inXSDDateTime ?dateTime .
-  BIND (YEAR(?dateTime) AS ?year)
-  ?event &lt;hasPopulationCount&gt; ?populationCount .
-  ?event &lt;concerns&gt; ?enslavedPeople .
-  ?enslavedPeople rdf:type &lt;EnslavedPeople&gt; .
+  ?event rdf:type/rdfs:subClassOf* &lt;http://example.org/Event&gt; .
+  ?event providesParticipantRole ?participantRoleRecord .
+  ?participantRoleRecord rdf:type/rdfs:subClassOf* &lt;http://example.org/ParticipantRoleRecord&gt; .
+  ?participantRoleRecord hasParticipantRoleType "enslaved" .  # Assuming "enslaved" is how enslaved people are identified
+  ?event hasTemporalExtent ?temporalExtent .
+  ?temporalExtent contains ?year . # Assuming year is represented as a date within the temporal extent
+  ?event hasName ?place . # Assuming the event has a name indicating the place
+  ?participantRoleRecord hasValue ?populationCount . # Assuming population count is directly attached to the role record
 }
 ```</t>
   </si>
@@ -382,35 +423,16 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?place ?year ?populationCount\nWHERE {\n  ?event rdf:type &lt;Event&gt; .\n  ?event &lt;hasPlace&gt; ?place .\n  ?event time:hasTime ?temporalEntity .\n  ?temporalEntity time:hasBeginning ?timeInstant .\n  ?timeInstant time:inXSDDateTime ?dateTime .\n  BIND (YEAR(?dateTime) AS ?year)\n  ?event &lt;hasPopulationCount&gt; ?populationCount .\n  ?event &lt;concerns&gt; ?enslavedPeople .\n  ?enslavedPeople rdf:type &lt;EnslavedPeople&gt; .\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?place ?year ?populationCount\nWHERE {\n  ?event rdf:type/rdfs:subClassOf* &lt;http://example.org/Event&gt; .\n  ?event providesParticipantRole ?participantRoleRecord .\n  ?participantRoleRecord rdf:type/rdfs:subClassOf* &lt;http://example.org/ParticipantRoleRecord&gt; .\n  ?participantRoleRecord hasParticipantRoleType \"enslaved\" .  # Assuming \"enslaved\" is how enslaved people are identified\n\n  ?event hasTemporalExtent ?temporalExtent .\n  ?temporalExtent contains ?year . # Assuming year is represented as a date within the temporal extent\n\n  ?event hasName ?place . # Assuming the event has a name indicating the place\n\n  ?participantRoleRecord hasValue ?populationCount . # Assuming population count is directly attached to the role record\n}\n```"
                     }
                 ],
                 "role": "model"
             },
-            "citation_metadata": {
-                "citations": [
-                    {
-                        "end_index": 166,
-                        "license": "BSD-3-Clause",
-                        "publication_date": null,
-                        "start_index": 10,
-                        "title": null,
-                        "uri": "https://github.com/RDFLib/rdflib"
-                    },
-                    {
-                        "end_index": 214,
-                        "license": null,
-                        "publication_date": null,
-                        "start_index": 46,
-                        "title": null,
-                        "uri": "https://github.com/IBM/AMR-CSLogic"
-                    }
-                ]
-            },
+            "citation_metadata": null,
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.03433514449555995,
+            "avg_logprobs": -0.11704982889109644,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -424,24 +446,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 236,
+        "candidates_token_count": 290,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 236
+                "token_count": 290
             }
         ],
-        "prompt_token_count": 675,
+        "prompt_token_count": 693,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 675
+                "token_count": 693
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 911
+        "total_token_count": 983
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -462,45 +484,49 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
@@ -508,8 +534,9 @@
 SELECT DISTINCT ?literacyStatus
 WHERE {
   ?agent a &lt;http://example.org/EnslavedIndividual&gt; .
-  ?agent &lt;http://example.org/hasLiteracyStatusRecord&gt; ?literacyStatusRecord .
-  ?literacyStatusRecord &lt;http://example.org/hasValue&gt; ?literacyStatus .
+  ?agentRecord a &lt;http://example.org/AgentRecord&gt; .
+  ?agent hasAgentRecord ?agentRecord .
+  ?agentRecord &lt;http://example.org/hasLiteracyStatus&gt; ?literacyStatus .
 }
 ```</t>
   </si>
@@ -528,7 +555,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT DISTINCT ?literacyStatus\nWHERE {\n  ?agent a &lt;http://example.org/EnslavedIndividual&gt; .\n  ?agent &lt;http://example.org/hasLiteracyStatusRecord&gt; ?literacyStatusRecord .\n  ?literacyStatusRecord &lt;http://example.org/hasValue&gt; ?literacyStatus .\n}\n```"
+                        "text": "```sparql\nSELECT DISTINCT ?literacyStatus\nWHERE {\n  ?agent a &lt;http://example.org/EnslavedIndividual&gt; .\n  ?agentRecord a &lt;http://example.org/AgentRecord&gt; .\n  ?agent hasAgentRecord ?agentRecord .\n  ?agentRecord &lt;http://example.org/hasLiteracyStatus&gt; ?literacyStatus .\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -537,7 +564,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.04480478733400755,
+            "avg_logprobs": -0.04245815390632266,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -551,24 +578,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 79,
+        "candidates_token_count": 84,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 79
+                "token_count": 84
             }
         ],
-        "prompt_token_count": 671,
+        "prompt_token_count": 689,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 671
+                "token_count": 689
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 750
+        "total_token_count": 773
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -589,54 +616,70 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT ?place ?relationshipType ?person
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+SELECT ?enslavedPerson ?place ?relationshipType
 WHERE {
-  ?person a &lt;http://example.org/EnslavedPerson&gt; .
-  ?person ?relationshipType ?place .
-  ?place a &lt;http://example.org/GeographicalPlace&gt; .
+  ?enslavedPerson rdf:type ?enslavedType .
+  ?enslavedType rdfs:subClassOf* &lt;http://example.org/Agent&gt; .  # Replace with the actual class for enslaved people if available
+  ?relationshipRecord a ?relationshipRecordType .
+  ?relationshipRecordType rdfs:subClassOf* &lt;http://example.org/AgentRecord&gt; .
+  ?relationshipRecord &lt;http://example.org/isRelationshipFrom&gt; ?enslavedPerson .  # Assuming this property links to the enslaved person
+  ?relationshipRecord &lt;http://example.org/isRelationshipTo&gt; ?place .   # Assuming this property links to a place
+  ?relationshipRecord &lt;http://example.org/hasInterAgentRelationshipType&gt; ?relationshipType . #Links the relationship record to its type.
+  ?place rdf:type ?placeType .
+  ?placeType rdfs:subClassOf* &lt;http://example.org/Agent&gt; . # Assuming places are also agents
+  FILTER EXISTS { ?enslavedPerson rdf:type &lt;http://example.org/enslaved&gt; }  # Example filter.  Replace with actual URI if available, otherwise remove.
+  FILTER EXISTS { ?place rdf:type &lt;http://example.org/GeographicalPlace&gt; }  # Example filter.  Replace with actual URI if available, otherwise remove.
 }
 ```</t>
   </si>
@@ -655,7 +698,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT ?place ?relationshipType ?person\nWHERE {\n  ?person a &lt;http://example.org/EnslavedPerson&gt; .\n  ?person ?relationshipType ?place .\n  ?place a &lt;http://example.org/GeographicalPlace&gt; .\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?enslavedPerson ?place ?relationshipType\nWHERE {\n  ?enslavedPerson rdf:type ?enslavedType .\n  ?enslavedType rdfs:subClassOf* &lt;http://example.org/Agent&gt; .  # Replace with the actual class for enslaved people if available\n\n  ?relationshipRecord a ?relationshipRecordType .\n  ?relationshipRecordType rdfs:subClassOf* &lt;http://example.org/AgentRecord&gt; .\n\n  ?relationshipRecord &lt;http://example.org/isRelationshipFrom&gt; ?enslavedPerson .  # Assuming this property links to the enslaved person\n  ?relationshipRecord &lt;http://example.org/isRelationshipTo&gt; ?place .   # Assuming this property links to a place\n\n  ?relationshipRecord &lt;http://example.org/hasInterAgentRelationshipType&gt; ?relationshipType . #Links the relationship record to its type.\n\n  ?place rdf:type ?placeType .\n  ?placeType rdfs:subClassOf* &lt;http://example.org/Agent&gt; . # Assuming places are also agents\n\n  FILTER EXISTS { ?enslavedPerson rdf:type &lt;http://example.org/enslaved&gt; }  # Example filter.  Replace with actual URI if available, otherwise remove.\n\n  FILTER EXISTS { ?place rdf:type &lt;http://example.org/GeographicalPlace&gt; }  # Example filter.  Replace with actual URI if available, otherwise remove.\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -664,7 +707,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.0759186139182439,
+            "avg_logprobs": -0.19091333270643315,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -678,24 +721,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 63,
+        "candidates_token_count": 418,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 63
+                "token_count": 418
             }
         ],
-        "prompt_token_count": 677,
+        "prompt_token_count": 695,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 677
+                "token_count": 695
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 740
+        "total_token_count": 1113
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -716,61 +759,75 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT DISTINCT ?firstName WHERE {
-  ?agent rdf:type Agent .
-  ?agent hasAgeRecord ?ageRecord .
-  ?ageRecord hasValue "Child" .
-  ?agent hasNameRecord ?nameRecord .
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+SELECT DISTINCT ?firstName
+WHERE {
+  ?agentRecord rdf:type ?ageRecordClass .
+  ?ageRecordClass rdfs:subClassOf* &lt;http://example.org/AgeRecord&gt; .
+  ?ageRecordClass rdfs:subClassOf* &lt;http://example.org/AgentRecord&gt; .
+  ?agent a &lt;http://example.org/Agent&gt; .
+  ?agent a ?enslavedType .
+  ?enslavedType rdfs:subClassOf* &lt;http://example.org/Agent&gt; .
+  ?enslavedType rdfs:label "Enslaved"@en .
+  ?agent hasAgentRecord ?agentRecord .
+  ?agent hasName ?nameRecord .
   ?nameRecord hasPreferredNameVariant ?nameVariant .
   ?nameVariant hasFirstnameAsString ?firstName .
-  ?ageRecord hasTemporalExtent ?temporalExtent .
-  ?temporalExtent rdf:type TIME:TemporalEntity .
-  ?temporalExtent TIME:hasBeginning ?begin .
-  ?temporalExtent TIME:hasEnd ?end .
-  FILTER (?begin &gt;= "1775-01-01"^^xsd:date &amp;&amp; ?end &lt;= "1783-12-31"^^xsd:date)
+  ?agentRecord hasTemporalExtent ?temporalExtent .
+  ?temporalExtent time:startsAt ?startDate .
+  FILTER (?startDate &gt;= "1775-01-01"^^xsd:date &amp;&amp; ?startDate &lt;= "1783-12-31"^^xsd:date) . #Revolutionary War dates
+  ?ageRecordClass hasAgeValue ?ageValue .
+  FILTER (?ageValue &lt; 18) .
 }
 ```</t>
   </si>
@@ -789,7 +846,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT DISTINCT ?firstName WHERE {\n  ?agent rdf:type Agent .\n  ?agent hasAgeRecord ?ageRecord .\n  ?ageRecord hasValue \"Child\" .\n  ?agent hasNameRecord ?nameRecord .\n  ?nameRecord hasPreferredNameVariant ?nameVariant .\n  ?nameVariant hasFirstnameAsString ?firstName .\n  ?ageRecord hasTemporalExtent ?temporalExtent .\n  ?temporalExtent rdf:type TIME:TemporalEntity .\n  ?temporalExtent TIME:hasBeginning ?begin .\n  ?temporalExtent TIME:hasEnd ?end .\n  FILTER (?begin &gt;= \"1775-01-01\"^^xsd:date &amp;&amp; ?end &lt;= \"1783-12-31\"^^xsd:date)\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT DISTINCT ?firstName\nWHERE {\n  ?agentRecord rdf:type ?ageRecordClass .\n  ?ageRecordClass rdfs:subClassOf* &lt;http://example.org/AgeRecord&gt; .\n  ?ageRecordClass rdfs:subClassOf* &lt;http://example.org/AgentRecord&gt; .\n  ?agent a &lt;http://example.org/Agent&gt; .\n  ?agent a ?enslavedType .\n  ?enslavedType rdfs:subClassOf* &lt;http://example.org/Agent&gt; .\n  ?enslavedType rdfs:label \"Enslaved\"@en .\n  ?agent hasAgentRecord ?agentRecord .\n  ?agent hasName ?nameRecord .\n  ?nameRecord hasPreferredNameVariant ?nameVariant .\n  ?nameVariant hasFirstnameAsString ?firstName .\n  ?agentRecord hasTemporalExtent ?temporalExtent .\n  ?temporalExtent time:startsAt ?startDate .\n  FILTER (?startDate &gt;= \"1775-01-01\"^^xsd:date &amp;&amp; ?startDate &lt;= \"1783-12-31\"^^xsd:date) . #Revolutionary War dates\n  ?ageRecordClass hasAgeValue ?ageValue .\n  FILTER (?ageValue &lt; 18) .\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -798,7 +855,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.019335713497428006,
+            "avg_logprobs": -0.0472230295186203,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -812,24 +869,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 172,
+        "candidates_token_count": 387,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 172
+                "token_count": 387
             }
         ],
-        "prompt_token_count": 675,
+        "prompt_token_count": 693,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 675
+                "token_count": 693
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 847
+        "total_token_count": 1080
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -850,64 +907,615 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT ?enslavedName ?enslaverName ?location WHERE {
-  ?interagentrecord a &lt;InterAgentRelationshipRecord&gt; .
-  ?interagentrecord &lt;hasInterAgentRelationshipType&gt; "enslaved by" .
-  ?interagentrecord &lt;isRelationshipTo&gt; ?enslaved .
-  ?enslaved &lt;hasNameRecord&gt; ?enslavedNameRecord .
-  ?enslavedNameRecord &lt;hasPreferredNameVariant&gt; ?enslavedNameVariant .
-  ?enslavedNameVariant &lt;fullNameAsString&gt; ?enslavedName .
-  ?interagentrecord &lt;isRelationshipFrom&gt; ?enslaver .
-  ?enslaver &lt;hasNameRecord&gt; ?enslaverNameRecord .
-  ?enslaverNameRecord &lt;hasPreferredNameVariant&gt; ?enslaverNameVariant .
-  ?enslaverNameVariant &lt;fullNameAsString&gt; ?enslaverName .
-  ?interagentrecord &lt;recordedAt&gt; ?event .
-  ?event &lt;hasPlace&gt; ?location .
-}
-```</t>
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+SELECT ?enslavedPerson ?enslaver ?event ?eventName WHERE {
+  ?enslavedPersonRoleRecord a ParticipantRoleRecord ;
+    hasParticipantRoleType "enslaved" .
+  ?event a Event ;
+    providesParticipantRole ?enslavedPersonRoleRecord .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?event providesParticipantRole ?enslaverRoleRecord .
+  ?enslaverRoleRecord hasParticipantRoleType "enslaver" .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .
+  ?enslaverRoleRecord roleProvidedBy ?event .
+  ?enslavedPersonRoleRecord roleProvidedBy ?event .</t>
   </si>
   <si>
     <t>{
@@ -924,7 +1532,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT ?enslavedName ?enslaverName ?location WHERE {\n  ?interagentrecord a &lt;InterAgentRelationshipRecord&gt; .\n  ?interagentrecord &lt;hasInterAgentRelationshipType&gt; \"enslaved by\" .\n  ?interagentrecord &lt;isRelationshipTo&gt; ?enslaved .\n  ?enslaved &lt;hasNameRecord&gt; ?enslavedNameRecord .\n  ?enslavedNameRecord &lt;hasPreferredNameVariant&gt; ?enslavedNameVariant .\n  ?enslavedNameVariant &lt;fullNameAsString&gt; ?enslavedName .\n  ?interagentrecord &lt;isRelationshipFrom&gt; ?enslaver .\n  ?enslaver &lt;hasNameRecord&gt; ?enslaverNameRecord .\n  ?enslaverNameRecord &lt;hasPreferredNameVariant&gt; ?enslaverNameVariant .\n  ?enslaverNameVariant &lt;fullNameAsString&gt; ?enslaverName .\n  ?interagentrecord &lt;recordedAt&gt; ?event .\n  ?event &lt;hasPlace&gt; ?location .\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?enslavedPerson ?enslaver ?event ?eventName WHERE {\n  ?enslavedPersonRoleRecord a ParticipantRoleRecord ;\n    hasParticipantRoleType \"enslaved\" .\n  ?event a Event ;\n    providesParticipantRole ?enslavedPersonRoleRecord .\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?event providesParticipantRole ?enslaverRoleRecord .\n  ?enslaverRoleRecord hasParticipantRoleType \"enslaver\" .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event .\n  ?enslaverRoleRecord roleProvidedBy ?event .\n\n  ?enslavedPersonRoleRecord roleProvidedBy ?event ."
                     }
                 ],
                 "role": "model"
@@ -932,8 +1540,8 @@
             "citation_metadata": null,
             "finish_message": null,
             "token_count": null,
-            "finish_reason": "STOP",
-            "avg_logprobs": -0.0467109260054937,
+            "finish_reason": "MAX_TOKENS",
+            "avg_logprobs": -0.0033317995257675648,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -947,24 +1555,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 227,
+        "candidates_token_count": 8192,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 227
+                "token_count": 8192
             }
         ],
-        "prompt_token_count": 674,
+        "prompt_token_count": 692,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 674
+                "token_count": 692
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 901
+        "total_token_count": 8884
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -985,62 +1593,69 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT DISTINCT ?childName
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+SELECT DISTINCT ?child
 WHERE {
-  ?relationshipRecord a InterAgentRelationshipRecord ;
-                        hasInterAgentRelationshipType "Parent-Child Relationship" .
-  ?relationshipRecord isRelationshipFrom ?parent .
+  ?relationshipRecord rdf:type InterAgentRelationshipRecord .
+  ?relationshipRecord hasInterAgentRelationshipType "ParentChildRelationship" .
+  ?relationshipRecord isRelationshipFrom ?enslaved .
   ?relationshipRecord isRelationshipTo ?child .
-  ?parent a Agent .
-  ?parent hasParticipantRoleRecord ?parentRoleRecord .
-  ?parentRoleRecord hasParticipantRoleType "Enslaved" .
-  ?child a Agent .
-  ?child hasNameRecord ?childNameRecord .
-  ?childNameRecord hasPreferredNameVariant ?childNameVariant .
-  ?childNameVariant fullNameAsString ?childName .
+  ?enslaved rdf:type ?agentType .
+  FILTER (?agentType != rdfs:Class)
+  ?enslaved ?hasAgentRecord ?agentRecord .
+  ?agentRecord rdf:type ?agentRecordType .
+  FILTER (?agentRecordType != rdfs:Class)
+  OPTIONAL{?agentRecord rdf:type OccupationRecord .
+           ?agentRecord hasValue "enslaved" .}
 }
 ```</t>
   </si>
@@ -1059,7 +1674,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT DISTINCT ?childName\nWHERE {\n  ?relationshipRecord a InterAgentRelationshipRecord ;\n                        hasInterAgentRelationshipType \"Parent-Child Relationship\" .\n  ?relationshipRecord isRelationshipFrom ?parent .\n  ?relationshipRecord isRelationshipTo ?child .\n  ?parent a Agent .\n  ?parent hasParticipantRoleRecord ?parentRoleRecord .\n  ?parentRoleRecord hasParticipantRoleType \"Enslaved\" .\n  ?child a Agent .\n  ?child hasNameRecord ?childNameRecord .\n  ?childNameRecord hasPreferredNameVariant ?childNameVariant .\n  ?childNameVariant fullNameAsString ?childName .\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\n\nSELECT DISTINCT ?child\nWHERE {\n  ?relationshipRecord rdf:type InterAgentRelationshipRecord .\n  ?relationshipRecord hasInterAgentRelationshipType \"ParentChildRelationship\" .\n  ?relationshipRecord isRelationshipFrom ?enslaved .\n  ?relationshipRecord isRelationshipTo ?child .\n  ?enslaved rdf:type ?agentType .\n  FILTER (?agentType != rdfs:Class)\n  ?enslaved ?hasAgentRecord ?agentRecord .\n  ?agentRecord rdf:type ?agentRecordType .\n  FILTER (?agentRecordType != rdfs:Class)\n  OPTIONAL{?agentRecord rdf:type OccupationRecord .\n           ?agentRecord hasValue \"enslaved\" .}\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -1068,7 +1683,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.07301585756499192,
+            "avg_logprobs": -0.07900218963623047,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -1082,24 +1697,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 145,
+        "candidates_token_count": 240,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 145
+                "token_count": 240
             }
         ],
-        "prompt_token_count": 670,
+        "prompt_token_count": 688,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 670
+                "token_count": 688
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 815
+        "total_token_count": 928
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -1120,63 +1735,69 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT DISTINCT ?agent
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+SELECT DISTINCT ?agentRecord
 WHERE {
-  ?agent rdf:type ?type .
-  FILTER (?type IN (
-    &lt;http://example.org/Enslaved&gt;,
-    &lt;http://example.org/FormerlyEnslaved&gt;
+  ?agentRecord rdf:type/rdfs:subClassOf* ?recordType .
+  FILTER (?recordType IN (
+    &lt;http://example.org/EnslavedRecord&gt;, 
+    &lt;http://example.org/FormerlyEnslavedRecord&gt;
   )) .
-  ?agent a &lt;http://example.org/Agent&gt; .
-  ?agent ?property ?record .
-  ?record recordedAt ?event .
-  ?event ?eventProperty ?location .
-  ?location rdf:type &lt;http://example.org/Location&gt; .
-  ?record hasTemporalExtent ?temporalExtent .
-  ?temporalExtent rdf:type &lt;http://example.org/TemporalExtent&gt; .
+  ?agentRecord recordedAt ?event .
+  ?event hasTemporalExtent ?temporalExtent .
+  ?temporalExtent contains ?date .
+  ?agentRecord recordedAt ?eventLocation .
+  ?eventLocation hasName ?locationName .
 }
 ```</t>
   </si>
@@ -1195,7 +1816,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT DISTINCT ?agent\nWHERE {\n  ?agent rdf:type ?type .\n  FILTER (?type IN (\n    &lt;http://example.org/Enslaved&gt;,\n    &lt;http://example.org/FormerlyEnslaved&gt;\n  )) .\n  ?agent a &lt;http://example.org/Agent&gt; .\n  ?agent ?property ?record .\n  ?record recordedAt ?event .\n  ?event ?eventProperty ?location .\n  ?location rdf:type &lt;http://example.org/Location&gt; .\n  ?record hasTemporalExtent ?temporalExtent .\n  ?temporalExtent rdf:type &lt;http://example.org/TemporalExtent&gt; .\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT DISTINCT ?agentRecord\nWHERE {\n  ?agentRecord rdf:type/rdfs:subClassOf* ?recordType .\n  FILTER (?recordType IN (\n    &lt;http://example.org/EnslavedRecord&gt;, \n    &lt;http://example.org/FormerlyEnslavedRecord&gt;\n  )) .\n  \n  ?agentRecord recordedAt ?event .\n  ?event hasTemporalExtent ?temporalExtent .\n  ?temporalExtent contains ?date .\n  \n  ?agentRecord recordedAt ?eventLocation .\n  ?eventLocation hasName ?locationName .\n  \n  \n}\n```"
                     }
                 ],
                 "role": "model"
@@ -1204,7 +1825,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.07888057808470882,
+            "avg_logprobs": -0.07242887488967704,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -1218,24 +1839,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 153,
+        "candidates_token_count": 239,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 153
+                "token_count": 239
             }
         ],
-        "prompt_token_count": 680,
+        "prompt_token_count": 698,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 680
+                "token_count": 698
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 833
+        "total_token_count": 937
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -1256,45 +1877,49 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
@@ -1303,15 +1928,22 @@
 PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
 PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
 PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
-SELECT DISTINCT ?child ?location ?timePeriod
+SELECT ?child ?location ?startDate ?endDate
 WHERE {
-  ?child rdf:type &lt;Agent&gt; .
-  ?child ?hasAgeRecordProperty ?ageRecord .
-  ?ageRecord rdf:type &lt;AgeRecord&gt; .
-  ?ageRecord &lt;hasValue&gt; "Child" .
-  ?ageRecord &lt;recordedAt&gt; ?event .
-  ?event ?locationProperty ?location .
-  ?ageRecord &lt;hasTemporalExtent&gt; ?timePeriod .
+  ?childRecord rdf:type ?ageRecordClass .
+  ?ageRecordClass rdfs:subClassOf* :AgentRecord .
+  ?childRecord a :AgeRecord .
+  ?childRecord :hasAgeValue ?age .
+  FILTER (?age &lt; 18) . 
+  ?agent a :Agent .
+  ?agent :hasAgentRecord ?childRecord .
+  ?childRecord :recordedAt ?event .
+  ?event :hasName ?location .
+  ?event :hasTemporalExtent ?temporalExtent .
+  ?temporalExtent time:startsAt ?startDate .
+  ?temporalExtent time:endsAt ?endDate .
+  FILTER EXISTS {?childRecord :providesParticipantRole ?role .
+                 ?role :hasParticipantRoleType "enslaved".}
 }
 ```</t>
   </si>
@@ -1330,35 +1962,16 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT DISTINCT ?child ?location ?timePeriod\nWHERE {\n  ?child rdf:type &lt;Agent&gt; .\n  ?child ?hasAgeRecordProperty ?ageRecord .\n  ?ageRecord rdf:type &lt;AgeRecord&gt; .\n  ?ageRecord &lt;hasValue&gt; \"Child\" .\n  ?ageRecord &lt;recordedAt&gt; ?event .\n  ?event ?locationProperty ?location .\n  ?ageRecord &lt;hasTemporalExtent&gt; ?timePeriod .\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?child ?location ?startDate ?endDate\nWHERE {\n  ?childRecord rdf:type ?ageRecordClass .\n  ?ageRecordClass rdfs:subClassOf* :AgentRecord .\n  ?childRecord a :AgeRecord .\n  ?childRecord :hasAgeValue ?age .\n  FILTER (?age &lt; 18) . \n  \n  ?agent a :Agent .\n  ?agent :hasAgentRecord ?childRecord .\n\n  ?childRecord :recordedAt ?event .\n  ?event :hasName ?location .\n  ?event :hasTemporalExtent ?temporalExtent .\n  ?temporalExtent time:startsAt ?startDate .\n  ?temporalExtent time:endsAt ?endDate .\n  \n  FILTER EXISTS {?childRecord :providesParticipantRole ?role .\n                 ?role :hasParticipantRoleType \"enslaved\".}\n}\n```"
                     }
                 ],
                 "role": "model"
             },
-            "citation_metadata": {
-                "citations": [
-                    {
-                        "end_index": 166,
-                        "license": "BSD-3-Clause",
-                        "publication_date": null,
-                        "start_index": 10,
-                        "title": null,
-                        "uri": "https://github.com/RDFLib/rdflib"
-                    },
-                    {
-                        "end_index": 214,
-                        "license": null,
-                        "publication_date": null,
-                        "start_index": 46,
-                        "title": null,
-                        "uri": "https://github.com/IBM/AMR-CSLogic"
-                    }
-                ]
-            },
+            "citation_metadata": null,
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.04086107908239687,
+            "avg_logprobs": -0.06622253676592293,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -1372,24 +1985,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 207,
+        "candidates_token_count": 295,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 207
+                "token_count": 295
             }
         ],
-        "prompt_token_count": 674,
+        "prompt_token_count": 692,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 674
+                "token_count": 692
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 881
+        "total_token_count": 987
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -1410,68 +2023,74 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT ?enslavedPerson (COUNT(DISTINCT ?enslavedPerson) AS ?numberOfEnslaved) WHERE {
-  ?owner a Agent .
-  ?relationshipRecord a InterAgentRelationshipRecord .
-  ?relationshipRecord isRelationshipFrom ?owner .
-  ?relationshipRecord isRelationshipTo ?enslavedPerson .
-  ?enslavedPerson a Agent .
-  ?relationshipRecord hasInterAgentRelationshipType "enslaved by" . # Assuming there is a relationship type defined for "enslaved by"
-  ?relationshipRecord recordedAt ?event .
-  ?event a Event .
-  # Optional: Add location and time constraints based on your data model
-  # Example:
-  # ?event hasPlace ?place .
-  # ?place a Place .
-  # ?place hasName "Specific Place" .
-  # ?event hasTime ?time .
-  # ?time time:hasBeginning ?beginning .
-  # ?beginning time:inXSDDate "Specific Date"^^xsd:date .
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+SELECT ?enslavedPerson ?owner ?event ?temporalExtent (COUNT(DISTINCT ?enslavedPerson) AS ?count) WHERE {
+  ?owner a &lt;Agent&gt; .
+  ?event a &lt;Event&gt; .
+  ?event providesParticipantRole ?participantRoleRecord .
+  ?participantRoleRecord hasParticipantRoleType "Owner" . # Assuming "Owner" is a valid ParticipantRoleType
+  ?participantRoleRecord roleProvidedBy ?event .
+  ?event hasTemporalExtent ?temporalExtent .
+  ?interAgentRelationshipRecord a &lt;InterAgentRelationshipRecord&gt; .
+  ?interAgentRelationshipRecord isRelationshipFrom ?owner .
+  ?interAgentRelationshipRecord isRelationshipTo ?enslavedPerson .
+  ?interAgentRelationshipRecord hasInterAgentRelationshipType "OwnerOf" . # Assuming "OwnerOf" represents the relationship
+  ?enslavedPerson a &lt;Agent&gt; .
+  FILTER EXISTS {
+    ?event &lt;hasName&gt; ?eventName . # Assuming events have name
+  }
+  GROUP BY ?enslavedPerson ?owner ?event ?temporalExtent
 }
-GROUP BY ?enslavedPerson
 ```</t>
   </si>
   <si>
@@ -1489,7 +2108,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT ?enslavedPerson (COUNT(DISTINCT ?enslavedPerson) AS ?numberOfEnslaved) WHERE {\n  ?owner a Agent .\n  ?relationshipRecord a InterAgentRelationshipRecord .\n  ?relationshipRecord isRelationshipFrom ?owner .\n  ?relationshipRecord isRelationshipTo ?enslavedPerson .\n  ?enslavedPerson a Agent .\n  ?relationshipRecord hasInterAgentRelationshipType \"enslaved by\" . # Assuming there is a relationship type defined for \"enslaved by\"\n  ?relationshipRecord recordedAt ?event .\n  ?event a Event .\n  # Optional: Add location and time constraints based on your data model\n  # Example:\n  # ?event hasPlace ?place .\n  # ?place a Place .\n  # ?place hasName \"Specific Place\" .\n  # ?event hasTime ?time .\n  # ?time time:hasBeginning ?beginning .\n  # ?beginning time:inXSDDate \"Specific Date\"^^xsd:date .\n}\nGROUP BY ?enslavedPerson\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?enslavedPerson ?owner ?event ?temporalExtent (COUNT(DISTINCT ?enslavedPerson) AS ?count) WHERE {\n  ?owner a &lt;Agent&gt; .\n  ?event a &lt;Event&gt; .\n  ?event providesParticipantRole ?participantRoleRecord .\n  ?participantRoleRecord hasParticipantRoleType \"Owner\" . # Assuming \"Owner\" is a valid ParticipantRoleType\n  ?participantRoleRecord roleProvidedBy ?event .\n  ?event hasTemporalExtent ?temporalExtent .\n  ?interAgentRelationshipRecord a &lt;InterAgentRelationshipRecord&gt; .\n  ?interAgentRelationshipRecord isRelationshipFrom ?owner .\n  ?interAgentRelationshipRecord isRelationshipTo ?enslavedPerson .\n  ?interAgentRelationshipRecord hasInterAgentRelationshipType \"OwnerOf\" . # Assuming \"OwnerOf\" represents the relationship\n  ?enslavedPerson a &lt;Agent&gt; .\n  FILTER EXISTS {\n    ?event &lt;hasName&gt; ?eventName . # Assuming events have name\n  }\n  \n  GROUP BY ?enslavedPerson ?owner ?event ?temporalExtent\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -1498,7 +2117,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.08785617957680912,
+            "avg_logprobs": -0.08519144142128506,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -1512,24 +2131,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 236,
+        "candidates_token_count": 341,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 236
+                "token_count": 341
             }
         ],
-        "prompt_token_count": 684,
+        "prompt_token_count": 702,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 684
+                "token_count": 702
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 920
+        "total_token_count": 1043
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -1550,59 +2169,70 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT ?enslavedPerson ?role
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt;
+SELECT ?enslavedIndividual ?role
 WHERE {
-  ?enslavedPerson a Agent .
-  ?enslavedPerson hasOccupationRecord ?occupationRecord .
-  ?occupationRecord hasValue "Enslaved" .
-  ?enslavedPerson hasParticipantRoleRecord ?participantRoleRecord .
-  ?participantRoleRecord hasParticipantRoleType ?role .
-  ?participantRoleRecord roleProvidedBy ?event .
-  ?event a &lt;http://example.org/ConstructionProject&gt; .
-  FILTER regex(str(?event), "state capitol", "i")
+  ?enslavedIndividualRecord a ?enslavedType .
+  ?enslavedType rdfs:subClassOf* &lt;http://example.org/AgentRecord&gt; .
+  ?enslavedIndividual &lt;http://example.org/hasAgentRecord&gt; ?enslavedIndividualRecord .
+  ?enslavedIndividualRecord &lt;http://example.org/recordedAt&gt; ?constructionEvent .
+  ?constructionEvent &lt;http://example.org/hasEventType&gt; ?eventType .
+  FILTER regex(str(?eventType), "construction", "i") .
+  ?constructionEvent &lt;http://example.org/providesParticipantRole&gt; ?participantRoleRecord .
+  ?participantRoleRecord &lt;http://example.org/hasParticipantRoleType&gt; ?role .
+  FILTER (contains(str(?role), "enslaved"))
+  FILTER (contains(str(?constructionEvent), "capitol") || contains(str(?constructionEvent), "Capitol"))
 }
 ```</t>
   </si>
@@ -1621,7 +2251,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT ?enslavedPerson ?role\nWHERE {\n  ?enslavedPerson a Agent .\n  ?enslavedPerson hasOccupationRecord ?occupationRecord .\n  ?occupationRecord hasValue \"Enslaved\" .\n  ?enslavedPerson hasParticipantRoleRecord ?participantRoleRecord .\n  ?participantRoleRecord hasParticipantRoleType ?role .\n  ?participantRoleRecord roleProvidedBy ?event .\n  ?event a &lt;http://example.org/ConstructionProject&gt; .\n  FILTER regex(str(?event), \"state capitol\", \"i\")\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\nPREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt;\n\nSELECT ?enslavedIndividual ?role\nWHERE {\n  ?enslavedIndividualRecord a ?enslavedType .\n  ?enslavedType rdfs:subClassOf* &lt;http://example.org/AgentRecord&gt; .\n  ?enslavedIndividual &lt;http://example.org/hasAgentRecord&gt; ?enslavedIndividualRecord .\n  ?enslavedIndividualRecord &lt;http://example.org/recordedAt&gt; ?constructionEvent .\n  ?constructionEvent &lt;http://example.org/hasEventType&gt; ?eventType .\n  FILTER regex(str(?eventType), \"construction\", \"i\") .\n  ?constructionEvent &lt;http://example.org/providesParticipantRole&gt; ?participantRoleRecord .\n  ?participantRoleRecord &lt;http://example.org/hasParticipantRoleType&gt; ?role .\n  FILTER (contains(str(?role), \"enslaved\"))\n  FILTER (contains(str(?constructionEvent), \"capitol\") || contains(str(?constructionEvent), \"Capitol\"))\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -1630,7 +2260,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.12800225546193678,
+            "avg_logprobs": -0.03808755436162839,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -1644,24 +2274,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 129,
+        "candidates_token_count": 348,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 129
+                "token_count": 348
             }
         ],
-        "prompt_token_count": 685,
+        "prompt_token_count": 703,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 685
+                "token_count": 703
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 814
+        "total_token_count": 1051
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -1682,61 +2312,62 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
-PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
-PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt;
-PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
-# There is no address or properties in the schema.
-# Returning empty result.
-SELECT DISTINCT ?addressOrProperty WHERE {
-  # Placeholder for a query that would retrieve address or property information.
-  # This query will always return an empty result set based on the current schema.
-  FILTER (false)  # This ensures no results are returned.
-  BIND("" AS ?addressOrProperty)
+SELECT DISTINCT ?address
+WHERE {
+  ?agent a/rdfs:subClassOf* Agent .
+  ?agentRecord a/rdfs:subClassOf* AgentRecord .
+  ?agent hasAgentRecord ?agentRecord .
+  ?agentRecord recordedAt ?event .
+  ?event providesParticipantRole ?roleRecord .
+  ?roleRecord hasParticipantRoleType "enslaved" .
+  ?event hasName ?address .
 }
 ```</t>
   </si>
@@ -1755,35 +2386,16 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\n# There is no address or properties in the schema.\n# Returning empty result.\nSELECT DISTINCT ?addressOrProperty WHERE {\n  # Placeholder for a query that would retrieve address or property information.\n  # This query will always return an empty result set based on the current schema.\n  FILTER (false)  # This ensures no results are returned.\n  BIND(\"\" AS ?addressOrProperty)\n}\n```"
+                        "text": "```sparql\nSELECT DISTINCT ?address\nWHERE {\n  ?agent a/rdfs:subClassOf* Agent .\n  ?agentRecord a/rdfs:subClassOf* AgentRecord .\n  ?agent hasAgentRecord ?agentRecord .\n  ?agentRecord recordedAt ?event .\n  ?event providesParticipantRole ?roleRecord .\n  ?roleRecord hasParticipantRoleType \"enslaved\" .\n  ?event hasName ?address .\n}\n```"
                     }
                 ],
                 "role": "model"
             },
-            "citation_metadata": {
-                "citations": [
-                    {
-                        "end_index": 166,
-                        "license": "BSD-3-Clause",
-                        "publication_date": null,
-                        "start_index": 10,
-                        "title": null,
-                        "uri": "https://github.com/RDFLib/rdflib"
-                    },
-                    {
-                        "end_index": 250,
-                        "license": "MIT",
-                        "publication_date": null,
-                        "start_index": 89,
-                        "title": null,
-                        "uri": "https://github.com/dpvcg/extract-sheets"
-                    }
-                ]
-            },
+            "citation_metadata": null,
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.17729352256669426,
+            "avg_logprobs": -0.06894138484325224,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -1797,24 +2409,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 217,
+        "candidates_token_count": 103,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 217
+                "token_count": 103
             }
         ],
-        "prompt_token_count": 675,
+        "prompt_token_count": 693,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 675
+                "token_count": 693
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 892
+        "total_token_count": 796
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -1835,59 +2447,79 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-# No specific schema provided to determine the properties related to enslavement, ports, transportation or temporal/demographic breakdowns.
-# Returning a query that will not return results.
-SELECT ?enslavedIndividual ?port ?time ?demographicBreakdown WHERE {
-  ?enslavedIndividual rdf:type ?EnslavedType . # Replace ?EnslavedType with the actual type for enslaved individuals
-  # Assuming there's a direct or indirect link to the port of embarkation
-  ?enslavedIndividual ?transportedFromProperty ?port . # Replace ?transportedFromProperty with the appropriate property
-  # Assuming there is a temporal property associated with the enslavement or transportation event
-  ?enslavedIndividual ?timeProperty ?time . # Replace ?timeProperty with the appropriate property
-  # Assuming there is a property that links to some demographic information
-  ?enslavedIndividual ?demographicProperty ?demographicBreakdown . # Replace ?demographicProperty with the appropriate property
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+SELECT ?enslavedPerson ?transportEvent ?temporalExtent ?sex ?age
+WHERE {
+  ?transportEvent rdf:type/rdfs:subClassOf* :Event .
+  ?transportEvent :hasEventType "Enslavement" .
+  ?transportEvent :providesParticipantRole ?participantRoleRecord .
+  ?participantRoleRecord :hasParticipantRoleType "EnslavedPerson" .
+  ?participantRoleRecord :roleProvidedBy ?transportEvent .
+  ?participantRoleRecord rdf:type :ParticipantRoleRecord .
+  ?enslavedPerson rdf:type :Agent .
+  ?enslavedPerson :hasAgentRecord ?participantRoleRecord .
+  ?transportEvent :hasTemporalExtent ?temporalExtent .
+  ?temporalExtent rdf:type :TemporalExtent .
+  OPTIONAL {
+    ?enslavedPerson :hasAgentRecord ?sexRecord .
+    ?sexRecord rdf:type :SexRecord .
+    ?sexRecord :hasValue ?sex .
+  }
+  OPTIONAL {
+    ?enslavedPerson :hasAgentRecord ?ageRecord .
+    ?ageRecord rdf:type :AgeRecord .
+    ?ageRecord :hasAgeValue ?age .
+  }
 }
 ```</t>
   </si>
@@ -1906,7 +2538,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\n# No specific schema provided to determine the properties related to enslavement, ports, transportation or temporal/demographic breakdowns.\n# Returning a query that will not return results.\nSELECT ?enslavedIndividual ?port ?time ?demographicBreakdown WHERE {\n  ?enslavedIndividual rdf:type ?EnslavedType . # Replace ?EnslavedType with the actual type for enslaved individuals\n\n  # Assuming there's a direct or indirect link to the port of embarkation\n  ?enslavedIndividual ?transportedFromProperty ?port . # Replace ?transportedFromProperty with the appropriate property\n\n  # Assuming there is a temporal property associated with the enslavement or transportation event\n  ?enslavedIndividual ?timeProperty ?time . # Replace ?timeProperty with the appropriate property\n\n  # Assuming there is a property that links to some demographic information\n  ?enslavedIndividual ?demographicProperty ?demographicBreakdown . # Replace ?demographicProperty with the appropriate property\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?enslavedPerson ?transportEvent ?temporalExtent ?sex ?age\nWHERE {\n  ?transportEvent rdf:type/rdfs:subClassOf* :Event .\n  ?transportEvent :hasEventType \"Enslavement\" .\n  ?transportEvent :providesParticipantRole ?participantRoleRecord .\n  ?participantRoleRecord :hasParticipantRoleType \"EnslavedPerson\" .\n  ?participantRoleRecord :roleProvidedBy ?transportEvent .\n  ?participantRoleRecord rdf:type :ParticipantRoleRecord .\n  ?enslavedPerson rdf:type :Agent .\n  ?enslavedPerson :hasAgentRecord ?participantRoleRecord .\n  \n  ?transportEvent :hasTemporalExtent ?temporalExtent .\n  ?temporalExtent rdf:type :TemporalExtent .\n  \n  OPTIONAL {\n    ?enslavedPerson :hasAgentRecord ?sexRecord .\n    ?sexRecord rdf:type :SexRecord .\n    ?sexRecord :hasValue ?sex .\n  }\n  OPTIONAL {\n    ?enslavedPerson :hasAgentRecord ?ageRecord .\n    ?ageRecord rdf:type :AgeRecord .\n    ?ageRecord :hasAgeValue ?age .\n  }\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -1915,7 +2547,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.29659430797283465,
+            "avg_logprobs": -0.03768590720924171,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -1929,24 +2561,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 208,
+        "candidates_token_count": 370,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 208
+                "token_count": 370
             }
         ],
-        "prompt_token_count": 677,
+        "prompt_token_count": 695,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 677
+                "token_count": 695
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 885
+        "total_token_count": 1065
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -1967,45 +2599,49 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
@@ -2014,17 +2650,24 @@
 PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
 PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
 PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
-SELECT DISTINCT ?rebellion ?participant ?location ?date WHERE {
-  ?rebellion rdf:type ?rebellionType .
-  ?rebellion rdfs:label ?rebellionName .
-  FILTER regex(str(?rebellionName), "rebellion", "i")
-  ?participantRoleRecord Event:providesParticipantRole ?rebellion .
-  ?participantRoleRecord Agent:hasParticipantRoleRecord ?participant .
-  ?participant rdfs:label ?participantName .
-  ?rebellion Event:hasTemporalExtent ?temporalExtent .
-  ?temporalExtent time:hasBeginning ?date .
-  ?rebellion Event:recordedAt ?location .
-  ?location rdfs:label ?locationName .
+SELECT ?rebellionName ?participant ?location ?startDate ?endDate
+WHERE {
+  ?rebellion rdf:type/rdfs:subClassOf* :Event .
+  ?rebellion :hasEventType "Slave Rebellion" .
+  ?rebellion :hasName ?rebellionName .
+  OPTIONAL {
+    ?rebellion :providesParticipantRole ?participantRoleRecord .
+    ?participantRoleRecord :subClassOf :AgentRecord .
+    ?participantRoleRecord :hasAgentRecord ?participant .
+  }
+  OPTIONAL {
+    ?rebellion :hasTemporalExtent ?temporalExtent .
+    ?temporalExtent :startsAt ?startDate .
+    ?temporalExtent :endsAt ?endDate .
+  }
+  OPTIONAL {
+   ?rebellion :hasLocation ?location .
+  }
 }
 ```</t>
   </si>
@@ -2043,35 +2686,16 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT DISTINCT ?rebellion ?participant ?location ?date WHERE {\n  ?rebellion rdf:type ?rebellionType .\n  ?rebellion rdfs:label ?rebellionName .\n  FILTER regex(str(?rebellionName), \"rebellion\", \"i\")\n\n  ?participantRoleRecord Event:providesParticipantRole ?rebellion .\n  ?participantRoleRecord Agent:hasParticipantRoleRecord ?participant .\n  ?participant rdfs:label ?participantName .\n\n  ?rebellion Event:hasTemporalExtent ?temporalExtent .\n  ?temporalExtent time:hasBeginning ?date .\n\n  ?rebellion Event:recordedAt ?location .\n  ?location rdfs:label ?locationName .\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?rebellionName ?participant ?location ?startDate ?endDate\nWHERE {\n  ?rebellion rdf:type/rdfs:subClassOf* :Event .\n  ?rebellion :hasEventType \"Slave Rebellion\" .\n  ?rebellion :hasName ?rebellionName .\n  OPTIONAL {\n    ?rebellion :providesParticipantRole ?participantRoleRecord .\n    ?participantRoleRecord :subClassOf :AgentRecord .\n    ?participantRoleRecord :hasAgentRecord ?participant .\n  }\n  OPTIONAL {\n    ?rebellion :hasTemporalExtent ?temporalExtent .\n    ?temporalExtent :startsAt ?startDate .\n    ?temporalExtent :endsAt ?endDate .\n  }\n  OPTIONAL {\n   ?rebellion :hasLocation ?location .\n  }\n}\n```"
                     }
                 ],
                 "role": "model"
             },
-            "citation_metadata": {
-                "citations": [
-                    {
-                        "end_index": 166,
-                        "license": "BSD-3-Clause",
-                        "publication_date": null,
-                        "start_index": 10,
-                        "title": null,
-                        "uri": "https://github.com/RDFLib/rdflib"
-                    },
-                    {
-                        "end_index": 214,
-                        "license": null,
-                        "publication_date": null,
-                        "start_index": 46,
-                        "title": null,
-                        "uri": "https://github.com/IBM/AMR-CSLogic"
-                    }
-                ]
-            },
+            "citation_metadata": null,
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.04921431154818148,
+            "avg_logprobs": -0.046602585332856765,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -2085,24 +2709,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 259,
+        "candidates_token_count": 278,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 259
+                "token_count": 278
             }
         ],
-        "prompt_token_count": 677,
+        "prompt_token_count": 695,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 677
+                "token_count": 695
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 936
+        "total_token_count": 973
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -2123,57 +2747,66 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT ?slave ?relative ?relationshipType ?location WHERE {
-  ?slave a :Agent .
-  ?slave :hasInterAgentRelationshipRecord ?relationshipRecord .
-  ?relationshipRecord :isRelationshipTo ?relative .
-  ?relationshipRecord :hasInterAgentRelationshipType ?relationshipType .
-  ?relationshipRecord :recordedAt ?event .
-  ?event :providesParticipantRole ?participantRoleRecord .
-  ?participantRoleRecord :roleProvidedBy ?location .
+SELECT ?slave ?slaveName ?relative ?relativeName ?relationshipType ?location WHERE {
+  ?slave a &lt;http://example.org/EnslavedIndividual&gt; .
+  ?slave &lt;http://example.org/hasName&gt; ?slaveName .
+  ?relationshipRecord &lt;http://example.org/isRelationshipFrom&gt; ?slave .
+  ?relationshipRecord &lt;http://example.org/isRelationshipTo&gt; ?relative .
+  ?relative &lt;http://example.org/hasName&gt; ?relativeName .
+  ?relationshipRecord &lt;http://example.org/hasInterAgentRelationshipType&gt; ?relationshipType .
+  OPTIONAL {
+    ?event &lt;http://example.org/providesParticipantRole&gt; ?roleRecord .
+    ?roleRecord &lt;http://example.org/hasParticipantRoleType&gt; ?locationRole .
+    FILTER (?locationRole = &lt;http://example.org/LocationRole&gt;) .
+    ?event &lt;http://example.org/hasName&gt; ?location .
+  }
 }
 ```</t>
   </si>
@@ -2192,7 +2825,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT ?slave ?relative ?relationshipType ?location WHERE {\n  ?slave a :Agent .\n  ?slave :hasInterAgentRelationshipRecord ?relationshipRecord .\n  ?relationshipRecord :isRelationshipTo ?relative .\n  ?relationshipRecord :hasInterAgentRelationshipType ?relationshipType .\n  ?relationshipRecord :recordedAt ?event .\n  ?event :providesParticipantRole ?participantRoleRecord .\n  ?participantRoleRecord :roleProvidedBy ?location .\n}\n```"
+                        "text": "```sparql\nSELECT ?slave ?slaveName ?relative ?relativeName ?relationshipType ?location WHERE {\n  ?slave a &lt;http://example.org/EnslavedIndividual&gt; .\n  ?slave &lt;http://example.org/hasName&gt; ?slaveName .\n  ?relationshipRecord &lt;http://example.org/isRelationshipFrom&gt; ?slave .\n  ?relationshipRecord &lt;http://example.org/isRelationshipTo&gt; ?relative .\n  ?relative &lt;http://example.org/hasName&gt; ?relativeName .\n  ?relationshipRecord &lt;http://example.org/hasInterAgentRelationshipType&gt; ?relationshipType .\n  OPTIONAL {\n    ?event &lt;http://example.org/providesParticipantRole&gt; ?roleRecord .\n    ?roleRecord &lt;http://example.org/hasParticipantRoleType&gt; ?locationRole .\n    FILTER (?locationRole = &lt;http://example.org/LocationRole&gt;) .\n    ?event &lt;http://example.org/hasName&gt; ?location .\n  }\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -2201,7 +2834,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.054568272716594195,
+            "avg_logprobs": -0.05702402785017684,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -2215,24 +2848,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 106,
+        "candidates_token_count": 222,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 106
+                "token_count": 222
             }
         ],
-        "prompt_token_count": 676,
+        "prompt_token_count": 694,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 676
+                "token_count": 694
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 782
+        "total_token_count": 916
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -2253,65 +2886,75 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT ?medianAge
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+PREFIX : &lt;https://example.org/&gt;
+SELECT (MEDIAN(?age) AS ?medianAge)
 WHERE {
-  ?agent rdf:type Agent .
-  ?agent :hasAgeRecord ?ageRecord .
-  ?ageRecord :hasAgeValue ?ageValue .
-  ?participantRoleRecord :roleProvidedBy ?event .
-  ?event rdf:type :Event .
-  ?participantRoleRecord :hasParticipantRoleType "enslaved" .
-  ?event :hasLocation "location X" .
-  ?event :hasTimePeriod "time period X" .
-  ?event rdf:type :EscapeEvent .  
-  # Calculate the median age (this is a simplified representation and may need adjustment based on the specific SPARQL engine and data distribution)
-  # This assumes you have a way to calculate the median age from the ?ageValue.  The following is a placeholder.
-  BIND(AVG(?ageValue) AS ?medianAge) # Replace AVG with the appropriate median calculation function if available.
+  ?escapeEvent a :Event ;
+               :hasEventType "Escape" .
+  ?escapeEvent :hasName ?location .
+  ?escapeEvent :hasTemporalExtent ?temporalExtent .
+  ?temporalExtent :startsAt ?startTime .
+  ?temporalExtent :endsAt ?endTime .
+  ?participantRoleRecord :roleProvidedBy ?escapeEvent ;
+                         :hasParticipantRoleType "EnslavedPerson" .
+  ?agentRecord :providesParticipantRole ?participantRoleRecord .
+  ?agentRecord a :AgeRecord ;
+               :hasAgeValue ?age .
+  FILTER (?location = "LocationX"^^xsd:string) .
+  FILTER (?startTime = "StartTimeX"^^xsd:date) .
+  FILTER (?endTime = "EndTimeX"^^xsd:date) .
 }
-GROUP BY ?event # Group by the event to ensure the median age is calculated within the context of each escape event.
 ```</t>
   </si>
   <si>
@@ -2329,7 +2972,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT ?medianAge\nWHERE {\n  ?agent rdf:type Agent .\n  ?agent :hasAgeRecord ?ageRecord .\n  ?ageRecord :hasAgeValue ?ageValue .\n  ?participantRoleRecord :roleProvidedBy ?event .\n  ?event rdf:type :Event .\n  ?participantRoleRecord :hasParticipantRoleType \"enslaved\" .\n  ?event :hasLocation \"location X\" .\n  ?event :hasTimePeriod \"time period X\" .\n  ?event rdf:type :EscapeEvent .  \n  \n  # Calculate the median age (this is a simplified representation and may need adjustment based on the specific SPARQL engine and data distribution)\n  # This assumes you have a way to calculate the median age from the ?ageValue.  The following is a placeholder.\n  BIND(AVG(?ageValue) AS ?medianAge) # Replace AVG with the appropriate median calculation function if available.\n}\nGROUP BY ?event # Group by the event to ensure the median age is calculated within the context of each escape event.\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\nPREFIX : &lt;https://example.org/&gt;\n\nSELECT (MEDIAN(?age) AS ?medianAge)\nWHERE {\n  ?escapeEvent a :Event ;\n               :hasEventType \"Escape\" .\n  ?escapeEvent :hasName ?location .\n  ?escapeEvent :hasTemporalExtent ?temporalExtent .\n  ?temporalExtent :startsAt ?startTime .\n  ?temporalExtent :endsAt ?endTime .\n\n  ?participantRoleRecord :roleProvidedBy ?escapeEvent ;\n                         :hasParticipantRoleType \"EnslavedPerson\" .\n  ?agentRecord :providesParticipantRole ?participantRoleRecord .\n  ?agentRecord a :AgeRecord ;\n               :hasAgeValue ?age .\n\n  FILTER (?location = \"LocationX\"^^xsd:string) .\n  FILTER (?startTime = \"StartTimeX\"^^xsd:date) .\n  FILTER (?endTime = \"EndTimeX\"^^xsd:date) .\n}\n\n```"
                     }
                 ],
                 "role": "model"
@@ -2338,7 +2981,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.2044022742738115,
+            "avg_logprobs": -0.06707161024261375,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -2352,24 +2995,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 235,
+        "candidates_token_count": 307,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 235
+                "token_count": 307
             }
         ],
-        "prompt_token_count": 679,
+        "prompt_token_count": 697,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 679
+                "token_count": 697
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 914
+        "total_token_count": 1004
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -2390,56 +3033,61 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT AVG(?age)
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+SELECT (AVG(?age) AS ?averageAgeAtDeath)
 WHERE {
-  ?agent a &lt;http://example.org/schema/Agent&gt; .
-  ?agent &lt;http://example.org/schema/hasAgeRecord&gt; ?ageRecord .
-  ?ageRecord &lt;http://example.org/schema/hasAgeValue&gt; ?age .
-  ?agent &lt;http://example.org/schema/hasParticipantRoleRecord&gt; ?roleRecord .
-  ?roleRecord &lt;http://example.org/schema/hasParticipantRoleType&gt; "enslaved" .
+  ?agentRecord rdf:type/rdfs:subClassOf* AgeRecord .
+  ?agentRecord hasAgeValue ?age .
 }
 ```</t>
   </si>
@@ -2458,7 +3106,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT AVG(?age)\nWHERE {\n  ?agent a &lt;http://example.org/schema/Agent&gt; .\n  ?agent &lt;http://example.org/schema/hasAgeRecord&gt; ?ageRecord .\n  ?ageRecord &lt;http://example.org/schema/hasAgeValue&gt; ?age .\n  ?agent &lt;http://example.org/schema/hasParticipantRoleRecord&gt; ?roleRecord .\n  ?roleRecord &lt;http://example.org/schema/hasParticipantRoleType&gt; \"enslaved\" .\n}\n```"
+                        "text": "```sparql\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT (AVG(?age) AS ?averageAgeAtDeath)\nWHERE {\n  ?agentRecord rdf:type/rdfs:subClassOf* AgeRecord .\n  ?agentRecord hasAgeValue ?age .\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -2467,7 +3115,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.07177248939138944,
+            "avg_logprobs": -0.03370567444832094,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -2481,24 +3129,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 122,
+        "candidates_token_count": 155,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 122
+                "token_count": 155
             }
         ],
-        "prompt_token_count": 672,
+        "prompt_token_count": 690,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 672
+                "token_count": 690
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 794
+        "total_token_count": 845
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -2519,45 +3167,49 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
@@ -2565,18 +3217,20 @@
 PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
 PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
 PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt;
 PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
-SELECT ?ethnicGroup ?skillCategory (COUNT(?agent) AS ?count) (SUM(?agentCount) / (SELECT COUNT(?totalAgent) FROM Agent AS ?totalCount) AS ?percentage) WHERE {
-  ?agent rdf:type Agent .
-  ?agent hasOccupationRecord ?occupationRecord .
-  ?occupationRecord hasValue ?skillCategory .
-  BIND("Ethnic Group Placeholder" AS ?ethnicGroup)
-  (SELECT (COUNT(?agentInner) AS ?agentCount) WHERE {
-    ?agentInner rdf:type Agent .
-    ?agentInner hasOccupationRecord ?occupationRecordInner .
-    ?occupationRecordInner hasValue ?skillCategoryInner .
-  } GROUP BY ?skillCategoryInner)
+SELECT ?ethnicGroup ?skillCategory (COUNT(?individual) AS ?count) (SUM(?individualCount) / (SELECT COUNT(DISTINCT ?totalIndividual) FROM {
+  ?totalIndividual rdf:type ?type .
+  ?type rdfs:subClassOf* &lt;http://example.org/EnslavedIndividual&gt; .
+}) AS ?percentage) WHERE {
+  ?individual rdf:type ?type .
+  ?type rdfs:subClassOf* &lt;http://example.org/EnslavedIndividual&gt; .
+  ?individual &lt;http://example.org/hasEthnicGroup&gt; ?ethnicGroup .
+  ?individual &lt;http://example.org/hasSkill&gt; ?skillCategory .
+  (SELECT (COUNT(?innerIndividual) AS ?individualCount) WHERE {
+   ?innerIndividual rdf:type ?innerType .
+   ?innerType rdfs:subClassOf* &lt;http://example.org/EnslavedIndividual&gt; .
+  }
+  )
 }
 GROUP BY ?ethnicGroup ?skillCategory
 ```</t>
@@ -2596,35 +3250,16 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?ethnicGroup ?skillCategory (COUNT(?agent) AS ?count) (SUM(?agentCount) / (SELECT COUNT(?totalAgent) FROM Agent AS ?totalCount) AS ?percentage) WHERE {\n  ?agent rdf:type Agent .\n  ?agent hasOccupationRecord ?occupationRecord .\n  ?occupationRecord hasValue ?skillCategory .\n  BIND(\"Ethnic Group Placeholder\" AS ?ethnicGroup)\n  (SELECT (COUNT(?agentInner) AS ?agentCount) WHERE {\n    ?agentInner rdf:type Agent .\n    ?agentInner hasOccupationRecord ?occupationRecordInner .\n    ?occupationRecordInner hasValue ?skillCategoryInner .\n  } GROUP BY ?skillCategoryInner)\n}\nGROUP BY ?ethnicGroup ?skillCategory\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?ethnicGroup ?skillCategory (COUNT(?individual) AS ?count) (SUM(?individualCount) / (SELECT COUNT(DISTINCT ?totalIndividual) FROM {\n  ?totalIndividual rdf:type ?type .\n  ?type rdfs:subClassOf* &lt;http://example.org/EnslavedIndividual&gt; .\n}) AS ?percentage) WHERE {\n  ?individual rdf:type ?type .\n  ?type rdfs:subClassOf* &lt;http://example.org/EnslavedIndividual&gt; .\n  ?individual &lt;http://example.org/hasEthnicGroup&gt; ?ethnicGroup .\n  ?individual &lt;http://example.org/hasSkill&gt; ?skillCategory .\n  (SELECT (COUNT(?innerIndividual) AS ?individualCount) WHERE {\n   ?innerIndividual rdf:type ?innerType .\n   ?innerType rdfs:subClassOf* &lt;http://example.org/EnslavedIndividual&gt; .\n  }\n  )\n}\nGROUP BY ?ethnicGroup ?skillCategory\n```"
                     }
                 ],
                 "role": "model"
             },
-            "citation_metadata": {
-                "citations": [
-                    {
-                        "end_index": 166,
-                        "license": "BSD-3-Clause",
-                        "publication_date": null,
-                        "start_index": 10,
-                        "title": null,
-                        "uri": "https://github.com/RDFLib/rdflib"
-                    },
-                    {
-                        "end_index": 250,
-                        "license": "MIT",
-                        "publication_date": null,
-                        "start_index": 89,
-                        "title": null,
-                        "uri": "https://github.com/dpvcg/extract-sheets"
-                    }
-                ]
-            },
+            "citation_metadata": null,
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.0783066831503537,
+            "avg_logprobs": -0.05674450258960782,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -2638,24 +3273,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 291,
+        "candidates_token_count": 327,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 291
+                "token_count": 327
             }
         ],
-        "prompt_token_count": 682,
+        "prompt_token_count": 700,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 682
+                "token_count": 700
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 973
+        "total_token_count": 1027
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -2676,45 +3311,49 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
@@ -2722,29 +3361,26 @@
 PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
 PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
 PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
-SELECT ?ethnicGroupingCategory (COUNT(?marriage) AS ?marriageCount) (xsd:decimal(COUNT(?marriage)) / xsd:decimal(SUM(COUNT(?marriage)) OVER ()) AS ?percentage)
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+PREFIX ex: &lt;http://example.org/&gt;
+SELECT ?ethnicGroupingType (COUNT(?marriageEvent) AS ?marriageCount) (SUM(IF(?sameEthnicGroup, 1, 0)) / COUNT(?marriageEvent) AS ?sameEthnicGroupPercentage)
 WHERE {
-  ?marriage a ?marriageType .
-  FILTER(REGEX(STR(?marriageType), "Marriage", "i"))
-  ?interAgentRelationshipRecord a ?interAgentRelationshipRecordType .
-  FILTER(REGEX(STR(?interAgentRelationshipRecordType), "InterAgentRelationshipRecord", "i"))
-  ?interAgentRelationshipRecord recordedAt ?marriage .
-  ?interAgentRelationshipRecord isRelationshipFrom ?slave1 .
-  ?interAgentRelationshipRecord isRelationshipTo ?slave2 .
-  ?slave1 hasNameRecord ?slave1NameRecord .
-  ?slave1NameRecord hasNameVariant ?slave1NameVariant .
-  OPTIONAL { ?slave1NameVariant hasSurnameAsString ?slave1Surname. }
-  OPTIONAL { ?slave1NameVariant hasFirstnameAsString ?slave1Firstname. }
-  ?slave2 hasNameRecord ?slave2NameRecord .
-  ?slave2NameRecord hasNameVariant ?slave2NameVariant .
-    OPTIONAL { ?slave2NameVariant hasSurnameAsString ?slave2Surname. }
-  OPTIONAL { ?slave2NameVariant hasFirstnameAsString ?slave2Firstname. }
-  BIND(IF((BOUND(?slave1Surname) &amp;&amp; BOUND(?slave2Surname) &amp;&amp; ?slave1Surname = ?slave2Surname) ||
-           (BOUND(?slave1Firstname) &amp;&amp; BOUND(?slave2Firstname) &amp;&amp; ?slave1Firstname = ?slave2Firstname),
-           "Same Ethnic Group", "Different Ethnic Groups") AS ?ethnicGroupingCategory)
+  ?marriageEvent rdf:type ex:Event .
+  ?marriageEvent ex:hasEventType "Marriage" .
+  ?marriageEvent ex:providesParticipantRole ?participantRole1 .
+  ?participantRole1 ex:hasParticipantRoleType "Husband" .
+  ?participantRole1 ex:subClassOf ex:AgentRecord .
+  ?participantRole1 ex:roleProvidedBy ?marriageEvent.
+  ?participantRole2 ex:hasParticipantRoleType "Wife" .
+  ?participantRole2 ex:subClassOf ex:AgentRecord .
+  ?participantRole2 ex:roleProvidedBy ?marriageEvent.
+  ?interAgentRelationshipRecord rdf:type ex:InterAgentRelationshipRecord .
+  ?interAgentRelationshipRecord ex:isRelationshipFrom ?participantRole1 .
+  ?interAgentRelationshipRecord ex:isRelationshipTo ?participantRole2 .
+  ?interAgentRelationshipRecord ex:hasInterAgentRelationshipType ?ethnicGroupingType .
+  BIND (IF(?ethnicGroupingType = "Same Ethnic Group", true, false) AS ?sameEthnicGroup)
 }
-GROUP BY ?ethnicGroupingCategory
-ORDER BY DESC(?marriageCount)
+GROUP BY ?ethnicGroupingType
 ```</t>
   </si>
   <si>
@@ -2762,27 +3398,16 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\n\nSELECT ?ethnicGroupingCategory (COUNT(?marriage) AS ?marriageCount) (xsd:decimal(COUNT(?marriage)) / xsd:decimal(SUM(COUNT(?marriage)) OVER ()) AS ?percentage)\nWHERE {\n  ?marriage a ?marriageType .\n  FILTER(REGEX(STR(?marriageType), \"Marriage\", \"i\"))\n\n  ?interAgentRelationshipRecord a ?interAgentRelationshipRecordType .\n  FILTER(REGEX(STR(?interAgentRelationshipRecordType), \"InterAgentRelationshipRecord\", \"i\"))\n  ?interAgentRelationshipRecord recordedAt ?marriage .\n  ?interAgentRelationshipRecord isRelationshipFrom ?slave1 .\n  ?interAgentRelationshipRecord isRelationshipTo ?slave2 .\n\n  ?slave1 hasNameRecord ?slave1NameRecord .\n  ?slave1NameRecord hasNameVariant ?slave1NameVariant .\n  OPTIONAL { ?slave1NameVariant hasSurnameAsString ?slave1Surname. }\n  OPTIONAL { ?slave1NameVariant hasFirstnameAsString ?slave1Firstname. }\n  \n  ?slave2 hasNameRecord ?slave2NameRecord .\n  ?slave2NameRecord hasNameVariant ?slave2NameVariant .\n    OPTIONAL { ?slave2NameVariant hasSurnameAsString ?slave2Surname. }\n  OPTIONAL { ?slave2NameVariant hasFirstnameAsString ?slave2Firstname. }\n\n  BIND(IF((BOUND(?slave1Surname) &amp;&amp; BOUND(?slave2Surname) &amp;&amp; ?slave1Surname = ?slave2Surname) ||\n           (BOUND(?slave1Firstname) &amp;&amp; BOUND(?slave2Firstname) &amp;&amp; ?slave1Firstname = ?slave2Firstname),\n           \"Same Ethnic Group\", \"Different Ethnic Groups\") AS ?ethnicGroupingCategory)\n}\nGROUP BY ?ethnicGroupingCategory\nORDER BY DESC(?marriageCount)\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\nPREFIX ex: &lt;http://example.org/&gt;\n\nSELECT ?ethnicGroupingType (COUNT(?marriageEvent) AS ?marriageCount) (SUM(IF(?sameEthnicGroup, 1, 0)) / COUNT(?marriageEvent) AS ?sameEthnicGroupPercentage)\nWHERE {\n  ?marriageEvent rdf:type ex:Event .\n  ?marriageEvent ex:hasEventType \"Marriage\" .\n\n  ?marriageEvent ex:providesParticipantRole ?participantRole1 .\n  ?participantRole1 ex:hasParticipantRoleType \"Husband\" .\n  ?participantRole1 ex:subClassOf ex:AgentRecord .\n  ?participantRole1 ex:roleProvidedBy ?marriageEvent.\n  \n  ?participantRole2 ex:hasParticipantRoleType \"Wife\" .\n  ?participantRole2 ex:subClassOf ex:AgentRecord .\n  ?participantRole2 ex:roleProvidedBy ?marriageEvent.\n\n  ?interAgentRelationshipRecord rdf:type ex:InterAgentRelationshipRecord .\n  ?interAgentRelationshipRecord ex:isRelationshipFrom ?participantRole1 .\n  ?interAgentRelationshipRecord ex:isRelationshipTo ?participantRole2 .\n  ?interAgentRelationshipRecord ex:hasInterAgentRelationshipType ?ethnicGroupingType .\n\n  BIND (IF(?ethnicGroupingType = \"Same Ethnic Group\", true, false) AS ?sameEthnicGroup)\n\n}\nGROUP BY ?ethnicGroupingType\n```"
                     }
                 ],
                 "role": "model"
             },
-            "citation_metadata": {
-                "citations": [
-                    {
-                        "end_index": 166,
-                        "license": "BSD-3-Clause",
-                        "publication_date": null,
-                        "start_index": 10,
-                        "title": null,
-                        "uri": "https://github.com/RDFLib/rdflib"
-                    }
-                ]
-            },
+            "citation_metadata": null,
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.07551177549155759,
+            "avg_logprobs": -0.05508178428367332,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -2796,24 +3421,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 462,
+        "candidates_token_count": 405,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 462
+                "token_count": 405
             }
         ],
-        "prompt_token_count": 683,
+        "prompt_token_count": 701,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 683
+                "token_count": 701
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 1145
+        "total_token_count": 1106
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -2834,62 +3459,76 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-# No specific schema available to fulfill this request. Returning a query with generic properties.
-# This query assumes the existence of properties like 'ethnicity', 'skills', 'gender', 'period', and 'economicValue' directly attached to individuals or through related entities.
-# Replace these generic properties with the actual properties in your knowledge graph.
-SELECT ?ethnicity ?skills ?gender ?period (SUM(?economicValue) AS ?totalEconomicValue)
-WHERE {
-  ?individual rdf:type dbo:EnslavedIndividual . # Assuming a class for enslaved individuals
-  OPTIONAL { ?individual ex:hasEthnicity ?ethnicity . } # Replace ex:hasEthnicity
-  OPTIONAL { ?individual ex:hasSkills ?skills . } # Replace ex:hasSkills
-  OPTIONAL { ?individual ex:hasGender ?gender . } # Replace ex:hasGender
-  OPTIONAL { ?individual ex:hasPeriod ?period . } # Replace ex:hasPeriod
-  ?individual ex:hasEconomicValue ?economicValue . # Replace ex:hasEconomicValue with the actual property
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+PREFIX example: &lt;http://example.org/&gt;
+SELECT ?ethnicity ?skill ?gender ?periodStart ?periodEnd ?economicValue WHERE {
+  ?agent rdf:type example:Agent .
+  OPTIONAL { ?agent example:hasAgentRecord ?ethnicityRecord .
+             ?ethnicityRecord rdf:type example:EthnicityRecord .
+             ?ethnicityRecord example:hasValue ?ethnicity . }
+  OPTIONAL { ?agent example:hasAgentRecord ?occupationRecord .
+             ?occupationRecord rdf:type example:OccupationRecord .
+             ?occupationRecord example:hasValue ?skill . }
+  OPTIONAL { ?agent example:hasAgentRecord ?sexRecord .
+             ?sexRecord rdf:type example:SexRecord .
+             ?sexRecord example:hasValue ?gender . }
+  OPTIONAL { ?agent example:hasAgentRecord ?economicValueRecord .
+             ?economicValueRecord rdf:type example:EconomicValueRecord .
+             ?economicValueRecord example:hasMonetaryValue ?economicValue .
+             ?economicValueRecord example:hasTemporalExtent ?temporalExtent .
+             ?temporalExtent time:startsAt ?periodStart .
+             ?temporalExtent time:endsAt ?periodEnd .}
 }
-GROUP BY ?ethnicity ?skills ?gender ?period
 ```</t>
   </si>
   <si>
@@ -2907,7 +3546,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\n# No specific schema available to fulfill this request. Returning a query with generic properties.\n# This query assumes the existence of properties like 'ethnicity', 'skills', 'gender', 'period', and 'economicValue' directly attached to individuals or through related entities.\n# Replace these generic properties with the actual properties in your knowledge graph.\nSELECT ?ethnicity ?skills ?gender ?period (SUM(?economicValue) AS ?totalEconomicValue)\nWHERE {\n  ?individual rdf:type dbo:EnslavedIndividual . # Assuming a class for enslaved individuals\n  OPTIONAL { ?individual ex:hasEthnicity ?ethnicity . } # Replace ex:hasEthnicity\n  OPTIONAL { ?individual ex:hasSkills ?skills . } # Replace ex:hasSkills\n  OPTIONAL { ?individual ex:hasGender ?gender . } # Replace ex:hasGender\n  OPTIONAL { ?individual ex:hasPeriod ?period . } # Replace ex:hasPeriod\n  ?individual ex:hasEconomicValue ?economicValue . # Replace ex:hasEconomicValue with the actual property\n\n}\nGROUP BY ?ethnicity ?skills ?gender ?period\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\nPREFIX example: &lt;http://example.org/&gt;\n\nSELECT ?ethnicity ?skill ?gender ?periodStart ?periodEnd ?economicValue WHERE {\n  ?agent rdf:type example:Agent .\n  OPTIONAL { ?agent example:hasAgentRecord ?ethnicityRecord .\n             ?ethnicityRecord rdf:type example:EthnicityRecord .\n             ?ethnicityRecord example:hasValue ?ethnicity . }\n  OPTIONAL { ?agent example:hasAgentRecord ?occupationRecord .\n             ?occupationRecord rdf:type example:OccupationRecord .\n             ?occupationRecord example:hasValue ?skill . }\n  OPTIONAL { ?agent example:hasAgentRecord ?sexRecord .\n             ?sexRecord rdf:type example:SexRecord .\n             ?sexRecord example:hasValue ?gender . }\n  OPTIONAL { ?agent example:hasAgentRecord ?economicValueRecord .\n             ?economicValueRecord rdf:type example:EconomicValueRecord .\n             ?economicValueRecord example:hasMonetaryValue ?economicValue .\n             ?economicValueRecord example:hasTemporalExtent ?temporalExtent .\n             ?temporalExtent time:startsAt ?periodStart .\n             ?temporalExtent time:endsAt ?periodEnd .}\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -2916,7 +3555,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.17166507898000724,
+            "avg_logprobs": -0.024828316432287157,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -2930,24 +3569,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 237,
+        "candidates_token_count": 361,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 237
+                "token_count": 361
             }
         ],
-        "prompt_token_count": 683,
+        "prompt_token_count": 701,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 683
+                "token_count": 701
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 920
+        "total_token_count": 1062
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -2968,62 +3607,69 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-# Assuming a class for enslaved individuals and a property linking them to events (e.g., life outcomes).
-# Also assuming a class for ships and a property linking them to agents (enslaved individuals).
 PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
 PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
-SELECT ?lifeOutcome
-WHERE {
-  ?ship rdf:type ShipClass .  # Replace ShipClass with the actual class for ships
-  ?enslavedIndividual rdf:type EnslavedIndividualClass . # Replace EnslavedIndividualClass with the actual class for enslaved individuals
-  ?enslavedIndividual ShipToEnslavedIndividualsProperty ?ship . # Replace ShipToEnslavedIndividualsProperty with the actual property linking ships to enslaved individuals
-  ?lifeOutcomeEvent rdf:type LifeOutcomeEventClass . # Replace LifeOutcomeEventClass with the actual class for life outcome events (e.g., sale, manumission, death)
-  ?enslavedIndividual LifeOutcomeEventProperty ?lifeOutcomeEvent . # Replace LifeOutcomeEventProperty with the actual property linking enslaved individuals to life outcome events
-  ?lifeOutcomeEvent rdfs:label ?lifeOutcome .  # Assuming life outcomes have labels
-  FILTER  (STR(?ship) = "XXX") # assumes ship is identified by its URI/ID
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+SELECT ?lifeOutcomeEventName WHERE {
+  ?ship rdf:type &lt;vocab:Ship&gt;.
+  ?ship a &lt;entity:XXX&gt;.
+  ?disembarkationEvent a &lt;vocab:DisembarkationEvent&gt; .
+  ?disembarkationEvent &lt;vocab:relatedToShip&gt; ?ship .
+  ?enslavedIndividualRoleRecord &lt;vocab:roleProvidedBy&gt; ?disembarkationEvent .
+  ?enslavedIndividualRoleRecord &lt;vocab:hasParticipantRoleType&gt; &lt;vocab:EnslavedIndividualRole&gt; .
+  ?enslavedIndividual &lt;vocab:hasAgentRecord&gt; ?enslavedIndividualRoleRecord .
+  ?lifeOutcomeEvent &lt;vocab:providesParticipantRole&gt; ?lifeOutcomeRoleRecord .
+  ?lifeOutcomeRoleRecord &lt;vocab:hasParticipantRoleType&gt; ?lifeOutcomeType .
+  ?lifeOutcomeRoleRecord &lt;vocab:roleProvidedBy&gt; ?lifeOutcomeEvent .
+  ?lifeOutcomeEvent &lt;vocab:hasName&gt; ?lifeOutcomeEventName . # Changed to get event name
+  ?lifeOutcomeRoleRecord &lt;vocab:agent&gt; ?enslavedIndividual .
 }
 ```</t>
   </si>
@@ -3042,7 +3688,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\n# Assuming a class for enslaved individuals and a property linking them to events (e.g., life outcomes).\n# Also assuming a class for ships and a property linking them to agents (enslaved individuals).\n\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\n\nSELECT ?lifeOutcome\nWHERE {\n  ?ship rdf:type ShipClass .  # Replace ShipClass with the actual class for ships\n  ?enslavedIndividual rdf:type EnslavedIndividualClass . # Replace EnslavedIndividualClass with the actual class for enslaved individuals\n  ?enslavedIndividual ShipToEnslavedIndividualsProperty ?ship . # Replace ShipToEnslavedIndividualsProperty with the actual property linking ships to enslaved individuals\n\n  ?lifeOutcomeEvent rdf:type LifeOutcomeEventClass . # Replace LifeOutcomeEventClass with the actual class for life outcome events (e.g., sale, manumission, death)\n  ?enslavedIndividual LifeOutcomeEventProperty ?lifeOutcomeEvent . # Replace LifeOutcomeEventProperty with the actual property linking enslaved individuals to life outcome events\n  ?lifeOutcomeEvent rdfs:label ?lifeOutcome .  # Assuming life outcomes have labels\n  FILTER  (STR(?ship) = \"XXX\") # assumes ship is identified by its URI/ID\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\n\nSELECT ?lifeOutcomeEventName WHERE {\n  ?ship rdf:type &lt;vocab:Ship&gt;.\n  ?ship a &lt;entity:XXX&gt;.\n  ?disembarkationEvent a &lt;vocab:DisembarkationEvent&gt; .\n  ?disembarkationEvent &lt;vocab:relatedToShip&gt; ?ship .\n  ?enslavedIndividualRoleRecord &lt;vocab:roleProvidedBy&gt; ?disembarkationEvent .\n  ?enslavedIndividualRoleRecord &lt;vocab:hasParticipantRoleType&gt; &lt;vocab:EnslavedIndividualRole&gt; .\n  ?enslavedIndividual &lt;vocab:hasAgentRecord&gt; ?enslavedIndividualRoleRecord .\n  \n  ?lifeOutcomeEvent &lt;vocab:providesParticipantRole&gt; ?lifeOutcomeRoleRecord .\n  ?lifeOutcomeRoleRecord &lt;vocab:hasParticipantRoleType&gt; ?lifeOutcomeType .\n  ?lifeOutcomeRoleRecord &lt;vocab:roleProvidedBy&gt; ?lifeOutcomeEvent .\n  ?lifeOutcomeEvent &lt;vocab:hasName&gt; ?lifeOutcomeEventName . # Changed to get event name\n  ?lifeOutcomeRoleRecord &lt;vocab:agent&gt; ?enslavedIndividual .\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -3051,7 +3697,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.18426466136706582,
+            "avg_logprobs": -0.12388206038635441,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -3065,24 +3711,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 321,
+        "candidates_token_count": 327,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 321
+                "token_count": 327
             }
         ],
-        "prompt_token_count": 688,
+        "prompt_token_count": 706,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 688
+                "token_count": 706
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 1009
+        "total_token_count": 1033
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -3103,62 +3749,71 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
 SELECT ?enslavedIndividual
 WHERE {
-  ?enslavedIndividual rdf:type :Agent .
-  ?enslavedIndividual :hasParticipantRoleRecord ?participantRoleRecord .
-  ?participantRoleRecord :hasParticipantRoleType "Enslaved" .
-  ?participantRoleRecord :recordedAt ?event .
-  ?event :hasLocation ?location .
-  ?location :name ?locationName .
-  FILTER (?locationName = "X") .
-  ?participantRoleRecord :hasTemporalExtent ?temporalExtent .
-  ?temporalExtent :begin ?beginTime .
-  ?temporalExtent :end ?endTime .
-  FILTER (?beginTime &lt;= "XXX"^^xsd:date &amp;&amp; ?endTime &gt;= "XXX"^^xsd:date)
+  ?enslavedIndividual rdf:type ?enslavedType .
+  ?enslavedType rdfs:subClassOf* &lt;http://example.org/Agent&gt; .  # Assuming Agent is the base class for individuals
+  ?enslavedIndividual ?locationProperty ?location .   # Assuming there is a location property to link to a location
+  FILTER regex(?location, "location X", "i")
+  ?agentRecord a ?recordType .
+  ?recordType rdfs:subClassOf* &lt;http://example.org/AgentRecord&gt; .
+  ?agentRecord rdf:type ?intermediateNode .
+  ?intermediateNode rdfs:subClassOf &lt;http://example.org/AgentRecord&gt; .
+  ?agentRecord hasTemporalExtent ?temporalExtent .
+  ?temporalExtent time:startsAt ?startTime .
+  ?temporalExtent time:endsAt ?endTime .
+  FILTER (?startTime &gt;= "XXX-01-01"^^xsd:date &amp;&amp; ?endTime &lt;= "XXX-12-31"^^xsd:date)
 }
 ```</t>
   </si>
@@ -3177,7 +3832,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT ?enslavedIndividual\nWHERE {\n  ?enslavedIndividual rdf:type :Agent .\n  ?enslavedIndividual :hasParticipantRoleRecord ?participantRoleRecord .\n  ?participantRoleRecord :hasParticipantRoleType \"Enslaved\" .\n  ?participantRoleRecord :recordedAt ?event .\n  ?event :hasLocation ?location .\n  ?location :name ?locationName .\n  FILTER (?locationName = \"X\") .\n  ?participantRoleRecord :hasTemporalExtent ?temporalExtent .\n  ?temporalExtent :begin ?beginTime .\n  ?temporalExtent :end ?endTime .\n  FILTER (?beginTime &lt;= \"XXX\"^^xsd:date &amp;&amp; ?endTime &gt;= \"XXX\"^^xsd:date)\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT ?enslavedIndividual\nWHERE {\n  ?enslavedIndividual rdf:type ?enslavedType .\n  ?enslavedType rdfs:subClassOf* &lt;http://example.org/Agent&gt; .  # Assuming Agent is the base class for individuals\n  ?enslavedIndividual ?locationProperty ?location .   # Assuming there is a location property to link to a location\n  FILTER regex(?location, \"location X\", \"i\")\n  ?agentRecord a ?recordType .\n  ?recordType rdfs:subClassOf* &lt;http://example.org/AgentRecord&gt; .\n  ?agentRecord rdf:type ?intermediateNode .\n  ?intermediateNode rdfs:subClassOf &lt;http://example.org/AgentRecord&gt; .\n  ?agentRecord hasTemporalExtent ?temporalExtent .\n  ?temporalExtent time:startsAt ?startTime .\n  ?temporalExtent time:endsAt ?endTime .\n  FILTER (?startTime &gt;= \"XXX-01-01\"^^xsd:date &amp;&amp; ?endTime &lt;= \"XXX-12-31\"^^xsd:date)\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -3186,7 +3841,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.04086910259156,
+            "avg_logprobs": -0.11839907196746476,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -3200,24 +3855,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 168,
+        "candidates_token_count": 348,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 168
+                "token_count": 348
             }
         ],
-        "prompt_token_count": 677,
+        "prompt_token_count": 695,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 677
+                "token_count": 695
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 845
+        "total_token_count": 1043
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -3238,67 +3893,82 @@
 Context:
 Below is the schema of a knowledge graph:
 Subject,Predicate,Object
-Agent,hasNameRecord,NameRecord
+Agent,hasAgentRecord,AgentRecord
+Agent,hasExternalReference,ExternalReference
+Agent,hasName,xsd:string
+AgentRecord,hasTemporalExtent,TemporalExtent
+AgentRecord,recordedAt,Event
+AgentRecord,temporalExtentContains,xsd:date
+AgeRecord,hasAgeValue,xsd:double
+AgeRecord,hasValue,AgeCategory.txt
+AgeRecord,subClassOf,AgentRecord
+Event,hasEventType,EventTypes.txt
+Event,hasExternalReference,ExternalReference
+Event,hasName,xsd:string
+Event,hasTemporalExtent,TemporalExtent
+Event,providesParticipantRole,ParticipantRoleRecord
+Event,subEventOf,Event
+ExternalReference,refersTo,ExternalReferent
+ExternalReference,withID,xsd:string
+InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
+InterAgentRelationshipRecord,isRelationshipFrom,Agent
+InterAgentRelationshipRecord,isRelationshipTo,Agent
+InterAgentRelationshipRecord,subClassOf,AgentRecord
+OccupationRecord,hasValue,Occupations.txt
+OccupationRecord,subClassOf,AgentRecord
+NameVariant,fullNameAsString,xsd:string
+NameVariant,hasFirstnameAsString,xsd:string
 NameRecord,hasNameVariant,NameVariant
 NameRecord,hasPreferredNameVariant,NameVariant
-NameVariant,fullNameAsString,xsd:string
 NameVariant,hasSurnameAsString,xsd:string
-NameVariant,hasFirstnameAsString,xsd:string
-NameVariant,isDirectlyBasedOn,EntityWithProvenance
-NameVariant,hasTemporalExtent,TemporalExtent
-NameVariant,recordedAt,Event
-Agent,hasSexRecord,SexRecord
+NameRecord,subClassOf,AgentRecord
+ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
+ParticipantRoleRecord,roleProvidedBy,Event
+ParticipantRoleRecord,subClassOf,AgentRecord
 SexRecord,hasValue,sexTypes.txt
-SexRecord,isDirectlyBasedOn,EntityWithProvenance
-SexRecord,hasTemporalExtent,TemporalExtent
-SexRecord,recordedAt,Event
-Agent,hasOccupationRecord,OccupationRecord
-OccupationRecord,hasValue,Occupations.txt
-OccupationRecord,isDirectlyBasedOn,EntityWithProvenance
-OccupationRecord,hasTemporalExtent,TemporalExtent
-OccupationRecord,recordedAt,Event
-Agent,hasAgeRecord,AgeRecord
-AgeRecord,hasValue,AgeCategory.txt
-AgeRecord,hasAgeValue,xsd:double
-AgeRecord,isDirectlyBasedOn,EntityWithProvenance
-AgeRecord,hasTemporalExtent,TemporalExtent
-AgeRecord,recordedAt,Event
-Agent,hasParticipantRoleRecord,ParticipantRoleRecord
-ParticipantRoleRecord,hasParticipantRoleType,ParticipantRoleTypes.txt
-ParticipantRoleRecord,isDirectlyBasedOn,EntityWithProvenance
-ParticipantRoleRecord,hasTemporalExtent,TemporalExtent
-ParticipantRoleRecord,recordedAt,Event
-ParticipantRoleRecord,roleProvidedBy,Event
-Event,providesParticipantRole,ParticipantRoleRecord
-Agent,hasInterAgentRelationshipRecord,InterAgentRelationshipRecord
-InterAgentRelationshipRecord,isRelationshipTo,Agent
-InterAgentRelationshipRecord,isRelationshipFrom,Agent
-InterAgentRelationshipRecord,hasInterAgentRelationshipType,InterAgentRelationshipTypes.txt
-InterAgentRelationshipRecord,isDirectlyBasedOn,EntityWithProvenance
-InterAgentRelationshipRecord,hasTemporalExtent,TemporalExtent
-InterAgentRelationshipRecord,recordedAt,Event
+SexRecord,subClassOf,AgentRecord
+TemporalExtent,contains,xsd:date
+TemporalExtent,endsAt,xsd:date
+TemporalExtent,fallsWithin,Timespan
+TemporalExtent,occursAfter,xsd:date
+TemporalExtent,occursBefore,xsd:date
+TemporalExtent,startsAt,xsd:date
+Timespan,endsAt,xsd:date
+Timespan,startsAt,xsd:date
+Timespan,subClassOf,TemporalExtent
 </t>
   </si>
   <si>
     <t>```sparql
-SELECT ?enslavedPerson ?name ?ownershipRecord ?ownershipEvent
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;
+PREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;
+PREFIX time: &lt;http://www.w3.org/2006/time#&gt;
+SELECT DISTINCT ?enslavedIndividual ?ownershipEvent ?ownershipRole
 WHERE {
-  # Find agents who have a participant role record indicating they were enslaved.
-  ?enslavedPerson a Agent ;
-                   hasParticipantRoleRecord ?enslavementRoleRecord .
-  ?enslavementRoleRecord hasParticipantRoleType "Enslaved" .
-  # Find agents who later have a participant role record indicating they were slave owners.
-  ?enslavedPerson hasParticipantRoleRecord ?ownershipRoleRecord .
-  ?ownershipRoleRecord hasParticipantRoleType "Slave Owner" .
-  ?ownershipRoleRecord recordedAt ?ownershipEvent .
-  #Get the name of the enslaved person
-  ?enslavedPerson hasNameRecord ?nameRecord .
-  ?nameRecord hasPreferredNameVariant ?nameVariant .
-  ?nameVariant fullNameAsString ?name .
-  # Optionally retrieve details about the ownership (the event where they were recorded as slave owners).
-  OPTIONAL {
-    ?ownershipRoleRecord isDirectlyBasedOn ?ownershipRecord .
-  }
+  # Find enslaved individuals
+  ?enslavedRoleRecord rdf:type ParticipantRoleRecord .
+  ?enslavedRoleRecord hasParticipantRoleType "enslaved" .
+  ?enslavedEvent rdf:type Event .
+  ?enslavedRoleRecord roleProvidedBy ?enslavedEvent .
+  ?enslavedEvent providesParticipantRole ?enslavedRoleRecord .
+  ?enslavedIndividualRecord rdf:type AgentRecord .
+  ?enslavedIndividualRecord recordedAt ?enslavedEvent .
+  ?enslavedIndividual a Agent ;
+   	  hasAgentRecord ?enslavedIndividualRecord .
+  # Find individuals who were slave owners
+  ?ownershipRoleRecord rdf:type ParticipantRoleRecord .
+  ?ownershipRoleRecord hasParticipantRoleType "slave owner" .
+  ?ownershipEvent rdf:type Event .
+  ?ownershipRoleRecord roleProvidedBy ?ownershipEvent .
+  ?ownershipEvent providesParticipantRole ?ownershipRoleRecord .
+  ?slaveOwnerIndividualRecord rdf:type AgentRecord .
+  ?slaveOwnerIndividualRecord recordedAt ?ownershipEvent .
+  ?slaveOwnerIndividual a Agent ;
+   	  hasAgentRecord ?slaveOwnerIndividualRecord .
+  # Ensure the enslaved individual is the same as the slave owner
+  FILTER (?enslavedIndividual = ?slaveOwnerIndividual)
+  BIND("slave owner" AS ?ownershipRole)
 }
 ```</t>
   </si>
@@ -3317,7 +3987,7 @@
                         "function_call": null,
                         "function_response": null,
                         "inline_data": null,
-                        "text": "```sparql\nSELECT ?enslavedPerson ?name ?ownershipRecord ?ownershipEvent\nWHERE {\n  # Find agents who have a participant role record indicating they were enslaved.\n  ?enslavedPerson a Agent ;\n                   hasParticipantRoleRecord ?enslavementRoleRecord .\n  ?enslavementRoleRecord hasParticipantRoleType \"Enslaved\" .\n\n  # Find agents who later have a participant role record indicating they were slave owners.\n  ?enslavedPerson hasParticipantRoleRecord ?ownershipRoleRecord .\n  ?ownershipRoleRecord hasParticipantRoleType \"Slave Owner\" .\n  ?ownershipRoleRecord recordedAt ?ownershipEvent .\n\n  #Get the name of the enslaved person\n  ?enslavedPerson hasNameRecord ?nameRecord .\n  ?nameRecord hasPreferredNameVariant ?nameVariant .\n  ?nameVariant fullNameAsString ?name .\n\n  # Optionally retrieve details about the ownership (the event where they were recorded as slave owners).\n  OPTIONAL {\n    ?ownershipRoleRecord isDirectlyBasedOn ?ownershipRecord .\n  }\n}\n```"
+                        "text": "```sparql\nPREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;\nPREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt;\nPREFIX xsd: &lt;http://www.w3.org/2001/XMLSchema#&gt;\nPREFIX time: &lt;http://www.w3.org/2006/time#&gt;\n\nSELECT DISTINCT ?enslavedIndividual ?ownershipEvent ?ownershipRole\nWHERE {\n  # Find enslaved individuals\n  ?enslavedRoleRecord rdf:type ParticipantRoleRecord .\n  ?enslavedRoleRecord hasParticipantRoleType \"enslaved\" .\n  ?enslavedEvent rdf:type Event .\n  ?enslavedRoleRecord roleProvidedBy ?enslavedEvent .\n  ?enslavedEvent providesParticipantRole ?enslavedRoleRecord .\n  ?enslavedIndividualRecord rdf:type AgentRecord .\n  ?enslavedIndividualRecord recordedAt ?enslavedEvent .\n  ?enslavedIndividual a Agent ;\n   \t  hasAgentRecord ?enslavedIndividualRecord .\n\n  # Find individuals who were slave owners\n  ?ownershipRoleRecord rdf:type ParticipantRoleRecord .\n  ?ownershipRoleRecord hasParticipantRoleType \"slave owner\" .\n  ?ownershipEvent rdf:type Event .\n  ?ownershipRoleRecord roleProvidedBy ?ownershipEvent .\n  ?ownershipEvent providesParticipantRole ?ownershipRoleRecord .\n  ?slaveOwnerIndividualRecord rdf:type AgentRecord .\n  ?slaveOwnerIndividualRecord recordedAt ?ownershipEvent .\n  ?slaveOwnerIndividual a Agent ;\n   \t  hasAgentRecord ?slaveOwnerIndividualRecord .\n  \n  # Ensure the enslaved individual is the same as the slave owner\n  FILTER (?enslavedIndividual = ?slaveOwnerIndividual)\n  \n  BIND(\"slave owner\" AS ?ownershipRole)\n}\n```"
                     }
                 ],
                 "role": "model"
@@ -3326,7 +3996,7 @@
             "finish_message": null,
             "token_count": null,
             "finish_reason": "STOP",
-            "avg_logprobs": -0.10028003316068854,
+            "avg_logprobs": -0.06420179069181145,
             "grounding_metadata": null,
             "index": null,
             "logprobs_result": null,
@@ -3340,24 +4010,24 @@
     "usage_metadata": {
         "cache_tokens_details": null,
         "cached_content_token_count": null,
-        "candidates_token_count": 233,
+        "candidates_token_count": 429,
         "candidates_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 233
+                "token_count": 429
             }
         ],
-        "prompt_token_count": 681,
+        "prompt_token_count": 699,
         "prompt_tokens_details": [
             {
                 "modality": "TEXT",
-                "token_count": 681
+                "token_count": 699
             }
         ],
         "thoughts_token_count": null,
         "tool_use_prompt_token_count": null,
         "tool_use_prompt_tokens_details": null,
-        "total_token_count": 914
+        "total_token_count": 1128
     },
     "automatic_function_calling_history": [],
     "parsed": null
@@ -3731,12 +4401,12 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="50.6640625" style="2" customWidth="1"/>
+    <col min="1" max="4" width="55" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">

</xml_diff>